<commit_message>
CIERRE 20 DIC 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/INVENTARIO ALMACEN  NOVIEMBRE        2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/INVENTARIO ALMACEN  NOVIEMBRE        2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="1215" windowWidth="18060" windowHeight="13620" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="7800" yWindow="1215" windowWidth="18060" windowHeight="13620" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ENERO  2021   " sheetId="1" r:id="rId1"/>
@@ -409,7 +409,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="109">
   <si>
     <t xml:space="preserve">INVENTARIO GENERAL </t>
   </si>
@@ -758,6 +758,30 @@
       <t xml:space="preserve">   DUPLICARON SALIDAS EN UNA CARGA DE PERNIL IBP</t>
     </r>
   </si>
+  <si>
+    <t>TAMPIQUEÑA</t>
+  </si>
+  <si>
+    <t>CABEZA DE LOM O</t>
+  </si>
+  <si>
+    <t>COSTILLA ESP DE CERDO</t>
+  </si>
+  <si>
+    <t>ATUN</t>
+  </si>
+  <si>
+    <t>MANTECA</t>
+  </si>
+  <si>
+    <t>BUCHE</t>
+  </si>
+  <si>
+    <t>TIENEN ERRORES</t>
+  </si>
+  <si>
+    <t>TIENEN ERROR  EN TOMA DE INVENTARIO  Y CAPTURA DE ALMANCEN</t>
+  </si>
 </sst>
 </file>
 
@@ -768,7 +792,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1044,6 +1068,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -1119,7 +1158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="74">
+  <borders count="77">
     <border>
       <left/>
       <right/>
@@ -2010,12 +2049,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="359">
+  <cellXfs count="390">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2583,9 +2667,6 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2697,6 +2778,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2876,6 +2967,68 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2886,10 +3039,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF99FF"/>
+      <color rgb="FFCC99FF"/>
+      <color rgb="FF0000FF"/>
       <color rgb="FFFF00FF"/>
-      <color rgb="FF0000FF"/>
       <color rgb="FF66FF66"/>
-      <color rgb="FFCC99FF"/>
       <color rgb="FF9966FF"/>
     </mruColors>
   </colors>
@@ -3233,10 +3387,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="299" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="299"/>
+      <c r="A1" s="304" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="304"/>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -3246,10 +3400,10 @@
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="300" t="s">
+      <c r="A2" s="305" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="301"/>
+      <c r="B2" s="306"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -3263,32 +3417,32 @@
     </row>
     <row r="3" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
-      <c r="B3" s="302" t="s">
+      <c r="B3" s="307" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="303"/>
+      <c r="C3" s="308"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="304" t="s">
+      <c r="E3" s="309" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="305"/>
+      <c r="F3" s="310"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="306" t="s">
+      <c r="H3" s="311" t="s">
         <v>2</v>
       </c>
       <c r="I3" s="11"/>
-      <c r="J3" s="313" t="s">
+      <c r="J3" s="318" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="314"/>
-      <c r="L3" s="309" t="s">
+      <c r="K3" s="319"/>
+      <c r="L3" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="310"/>
-      <c r="N3" s="311" t="s">
+      <c r="M3" s="315"/>
+      <c r="N3" s="316" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="312"/>
+      <c r="O3" s="317"/>
     </row>
     <row r="4" spans="1:15" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
@@ -3310,7 +3464,7 @@
       <c r="G4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="307"/>
+      <c r="H4" s="312"/>
       <c r="I4" s="11"/>
       <c r="J4" s="16" t="s">
         <v>10</v>
@@ -3583,10 +3737,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N11" s="315" t="s">
+      <c r="N11" s="320" t="s">
         <v>40</v>
       </c>
-      <c r="O11" s="316"/>
+      <c r="O11" s="321"/>
     </row>
     <row r="12" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
@@ -3756,10 +3910,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N16" s="317" t="s">
+      <c r="N16" s="322" t="s">
         <v>41</v>
       </c>
-      <c r="O16" s="318"/>
+      <c r="O16" s="323"/>
     </row>
     <row r="17" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
@@ -3836,10 +3990,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N18" s="319" t="s">
+      <c r="N18" s="324" t="s">
         <v>42</v>
       </c>
-      <c r="O18" s="320"/>
+      <c r="O18" s="325"/>
     </row>
     <row r="19" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
@@ -4335,10 +4489,10 @@
     <row r="34" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="70"/>
       <c r="C34" s="72"/>
-      <c r="E34" s="308" t="s">
+      <c r="E34" s="313" t="s">
         <v>34</v>
       </c>
-      <c r="F34" s="308"/>
+      <c r="F34" s="313"/>
       <c r="G34" s="73">
         <f>SUM(G5:G27)</f>
         <v>68686.460000000006</v>
@@ -4414,10 +4568,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="349" t="s">
+      <c r="B1" s="354" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="349"/>
+      <c r="C1" s="354"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -4429,15 +4583,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="300">
+      <c r="B2" s="305">
         <v>44507</v>
       </c>
-      <c r="C2" s="301"/>
-      <c r="F2" s="327" t="s">
+      <c r="C2" s="306"/>
+      <c r="F2" s="332" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="327"/>
-      <c r="H2" s="327"/>
+      <c r="G2" s="332"/>
+      <c r="H2" s="332"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -4447,32 +4601,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="302" t="s">
+      <c r="C3" s="307" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="303"/>
+      <c r="D3" s="308"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="304" t="s">
+      <c r="F3" s="309" t="s">
         <v>94</v>
       </c>
-      <c r="G3" s="305"/>
+      <c r="G3" s="310"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="306" t="s">
+      <c r="I3" s="311" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="313" t="s">
+      <c r="K3" s="318" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="314"/>
-      <c r="M3" s="309" t="s">
+      <c r="L3" s="319"/>
+      <c r="M3" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="310"/>
-      <c r="O3" s="311" t="s">
+      <c r="N3" s="315"/>
+      <c r="O3" s="316" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="312"/>
+      <c r="P3" s="317"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -4494,7 +4648,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="307"/>
+      <c r="I4" s="312"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -4543,16 +4697,16 @@
       <c r="L5" s="208">
         <v>5</v>
       </c>
-      <c r="M5" s="281">
+      <c r="M5" s="280">
         <f>K5-H5</f>
         <v>0</v>
       </c>
-      <c r="N5" s="282">
+      <c r="N5" s="281">
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="350"/>
-      <c r="P5" s="339"/>
+      <c r="O5" s="355"/>
+      <c r="P5" s="344"/>
     </row>
     <row r="6" spans="2:24" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -4582,16 +4736,16 @@
       <c r="L6" s="208">
         <v>57</v>
       </c>
-      <c r="M6" s="283">
+      <c r="M6" s="282">
         <f t="shared" ref="M6:N22" si="2">K6-H6</f>
         <v>0</v>
       </c>
-      <c r="N6" s="284">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="351"/>
-      <c r="P6" s="331"/>
+      <c r="N6" s="283">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="356"/>
+      <c r="P6" s="336"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
       <c r="U6" s="226"/>
@@ -4627,11 +4781,11 @@
       <c r="L7" s="208">
         <v>21</v>
       </c>
-      <c r="M7" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N7" s="286">
+      <c r="M7" s="284">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="285">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4658,16 +4812,16 @@
       <c r="J8" s="28"/>
       <c r="K8" s="207"/>
       <c r="L8" s="208"/>
-      <c r="M8" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="348"/>
-      <c r="P8" s="343"/>
+      <c r="M8" s="284">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="353"/>
+      <c r="P8" s="348"/>
     </row>
     <row r="9" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="21" t="s">
@@ -4697,15 +4851,15 @@
       <c r="L9" s="208">
         <v>9</v>
       </c>
-      <c r="M9" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N9" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="261"/>
+      <c r="M9" s="284">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="260"/>
       <c r="P9" s="132"/>
     </row>
     <row r="10" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4736,16 +4890,16 @@
       <c r="L10" s="208">
         <v>9</v>
       </c>
-      <c r="M10" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N10" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="352"/>
-      <c r="P10" s="333"/>
+      <c r="M10" s="284">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="357"/>
+      <c r="P10" s="338"/>
     </row>
     <row r="11" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="164" t="s">
@@ -4775,15 +4929,15 @@
       <c r="L11" s="208">
         <v>317</v>
       </c>
-      <c r="M11" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="262"/>
+      <c r="M11" s="284">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="261"/>
       <c r="P11" s="239"/>
     </row>
     <row r="12" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4814,15 +4968,15 @@
       <c r="L12" s="213">
         <v>28</v>
       </c>
-      <c r="M12" s="285">
+      <c r="M12" s="284">
         <f t="shared" si="2"/>
         <v>-4.0400000000000773</v>
       </c>
-      <c r="N12" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="263"/>
+      <c r="N12" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="262"/>
       <c r="P12" s="136"/>
     </row>
     <row r="13" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4853,15 +5007,15 @@
       <c r="L13" s="213">
         <v>247</v>
       </c>
-      <c r="M13" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="264"/>
+      <c r="M13" s="284">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="263"/>
       <c r="P13" s="138"/>
     </row>
     <row r="14" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4892,16 +5046,16 @@
       <c r="L14" s="213">
         <v>20</v>
       </c>
-      <c r="M14" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="353"/>
-      <c r="P14" s="322"/>
+      <c r="M14" s="284">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="358"/>
+      <c r="P14" s="327"/>
     </row>
     <row r="15" spans="2:24" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="21" t="s">
@@ -4923,15 +5077,15 @@
       <c r="J15" s="28"/>
       <c r="K15" s="212"/>
       <c r="L15" s="213"/>
-      <c r="M15" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="265"/>
+      <c r="M15" s="284">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="264"/>
       <c r="P15" s="140"/>
     </row>
     <row r="16" spans="2:24" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4954,15 +5108,15 @@
       <c r="J16" s="28"/>
       <c r="K16" s="212"/>
       <c r="L16" s="213"/>
-      <c r="M16" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="266"/>
+      <c r="M16" s="284">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="265"/>
       <c r="P16" s="142"/>
     </row>
     <row r="17" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4985,15 +5139,15 @@
       <c r="J17" s="28"/>
       <c r="K17" s="212"/>
       <c r="L17" s="213"/>
-      <c r="M17" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="267"/>
+      <c r="M17" s="284">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="266"/>
       <c r="P17" s="144"/>
     </row>
     <row r="18" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5024,15 +5178,15 @@
       <c r="L18" s="213">
         <v>507</v>
       </c>
-      <c r="M18" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="268"/>
+      <c r="M18" s="284">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="267"/>
       <c r="P18" s="146"/>
     </row>
     <row r="19" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5055,16 +5209,16 @@
       <c r="J19" s="5"/>
       <c r="K19" s="212"/>
       <c r="L19" s="213"/>
-      <c r="M19" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="354"/>
-      <c r="P19" s="324"/>
+      <c r="M19" s="284">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="359"/>
+      <c r="P19" s="329"/>
     </row>
     <row r="20" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="21" t="s">
@@ -5086,15 +5240,15 @@
       <c r="J20" s="28"/>
       <c r="K20" s="212"/>
       <c r="L20" s="213"/>
-      <c r="M20" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="269"/>
+      <c r="M20" s="284">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="268"/>
       <c r="P20" s="148"/>
     </row>
     <row r="21" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5125,16 +5279,16 @@
       <c r="L21" s="213">
         <v>180</v>
       </c>
-      <c r="M21" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="286">
+      <c r="M21" s="284">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="285">
         <f t="shared" si="2"/>
         <v>162</v>
       </c>
-      <c r="O21" s="355"/>
-      <c r="P21" s="329"/>
+      <c r="O21" s="360"/>
+      <c r="P21" s="334"/>
     </row>
     <row r="22" spans="2:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
@@ -5164,16 +5318,16 @@
       <c r="L22" s="213">
         <v>1212</v>
       </c>
-      <c r="M22" s="287">
+      <c r="M22" s="286">
         <f t="shared" si="2"/>
         <v>-4.0000000000873115E-2</v>
       </c>
-      <c r="N22" s="288">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="356"/>
-      <c r="P22" s="357"/>
+      <c r="N22" s="287">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="361"/>
+      <c r="P22" s="362"/>
     </row>
     <row r="23" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="21" t="s">
@@ -5203,15 +5357,15 @@
       <c r="L23" s="217">
         <v>43</v>
       </c>
-      <c r="M23" s="285">
+      <c r="M23" s="284">
         <f t="shared" ref="M23:N36" si="3">K23-H23</f>
         <v>-0.75</v>
       </c>
-      <c r="N23" s="286">
+      <c r="N23" s="285">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O23" s="270"/>
+      <c r="O23" s="269"/>
       <c r="P23" s="192"/>
     </row>
     <row r="24" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5234,15 +5388,15 @@
       <c r="J24" s="28"/>
       <c r="K24" s="216"/>
       <c r="L24" s="217"/>
-      <c r="M24" s="285">
+      <c r="M24" s="284">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N24" s="286">
+      <c r="N24" s="285">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O24" s="271"/>
+      <c r="O24" s="270"/>
       <c r="P24" s="194"/>
     </row>
     <row r="25" spans="2:16" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5265,16 +5419,16 @@
       <c r="J25" s="28"/>
       <c r="K25" s="218"/>
       <c r="L25" s="213"/>
-      <c r="M25" s="289">
+      <c r="M25" s="288">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N25" s="290">
+      <c r="N25" s="289">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O25" s="358"/>
-      <c r="P25" s="337"/>
+      <c r="O25" s="363"/>
+      <c r="P25" s="342"/>
     </row>
     <row r="26" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="21" t="s">
@@ -5296,15 +5450,15 @@
       <c r="J26" s="28"/>
       <c r="K26" s="218"/>
       <c r="L26" s="213"/>
-      <c r="M26" s="291">
+      <c r="M26" s="290">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N26" s="292">
+      <c r="N26" s="291">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O26" s="272"/>
+      <c r="O26" s="271"/>
       <c r="P26" s="196"/>
     </row>
     <row r="27" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5335,15 +5489,15 @@
       <c r="L27" s="213">
         <v>17</v>
       </c>
-      <c r="M27" s="291">
+      <c r="M27" s="290">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N27" s="292">
+      <c r="N27" s="291">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O27" s="273"/>
+      <c r="O27" s="272"/>
       <c r="P27" s="96"/>
     </row>
     <row r="28" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5366,15 +5520,15 @@
       <c r="J28" s="28"/>
       <c r="K28" s="218"/>
       <c r="L28" s="213"/>
-      <c r="M28" s="291">
+      <c r="M28" s="290">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N28" s="292">
+      <c r="N28" s="291">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O28" s="273"/>
+      <c r="O28" s="272"/>
       <c r="P28" s="96"/>
     </row>
     <row r="29" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5397,15 +5551,15 @@
       <c r="J29" s="28"/>
       <c r="K29" s="218"/>
       <c r="L29" s="213"/>
-      <c r="M29" s="291">
+      <c r="M29" s="290">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N29" s="292">
+      <c r="N29" s="291">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O29" s="274"/>
+      <c r="O29" s="273"/>
       <c r="P29" s="98"/>
     </row>
     <row r="30" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5428,15 +5582,15 @@
       <c r="J30" s="28"/>
       <c r="K30" s="218"/>
       <c r="L30" s="213"/>
-      <c r="M30" s="291">
+      <c r="M30" s="290">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N30" s="292">
+      <c r="N30" s="291">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O30" s="275"/>
+      <c r="O30" s="274"/>
       <c r="P30" s="93"/>
     </row>
     <row r="31" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5459,15 +5613,15 @@
       <c r="J31" s="28"/>
       <c r="K31" s="218"/>
       <c r="L31" s="213"/>
-      <c r="M31" s="291">
+      <c r="M31" s="290">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N31" s="292">
+      <c r="N31" s="291">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O31" s="276"/>
+      <c r="O31" s="275"/>
       <c r="P31" s="100"/>
     </row>
     <row r="32" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5490,15 +5644,15 @@
       <c r="J32" s="28"/>
       <c r="K32" s="218"/>
       <c r="L32" s="213"/>
-      <c r="M32" s="293">
+      <c r="M32" s="292">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N32" s="294">
+      <c r="N32" s="293">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O32" s="277"/>
+      <c r="O32" s="276"/>
       <c r="P32" s="198"/>
     </row>
     <row r="33" spans="2:16" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5521,15 +5675,15 @@
       <c r="J33" s="28"/>
       <c r="K33" s="218"/>
       <c r="L33" s="213"/>
-      <c r="M33" s="289">
+      <c r="M33" s="288">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N33" s="290">
+      <c r="N33" s="289">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O33" s="278"/>
+      <c r="O33" s="277"/>
       <c r="P33" s="232"/>
     </row>
     <row r="34" spans="2:16" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
@@ -5552,15 +5706,15 @@
       <c r="J34" s="28"/>
       <c r="K34" s="43"/>
       <c r="L34" s="121"/>
-      <c r="M34" s="295">
+      <c r="M34" s="294">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N34" s="296">
+      <c r="N34" s="295">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O34" s="279"/>
+      <c r="O34" s="278"/>
       <c r="P34" s="200"/>
     </row>
     <row r="35" spans="2:16" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -5583,15 +5737,15 @@
       <c r="J35" s="28"/>
       <c r="K35" s="43"/>
       <c r="L35" s="121"/>
-      <c r="M35" s="295">
+      <c r="M35" s="294">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N35" s="296">
+      <c r="N35" s="295">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O35" s="276"/>
+      <c r="O35" s="275"/>
       <c r="P35" s="100"/>
     </row>
     <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5612,24 +5766,24 @@
       <c r="J36" s="28"/>
       <c r="K36" s="69"/>
       <c r="L36" s="179"/>
-      <c r="M36" s="297">
+      <c r="M36" s="296">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N36" s="298">
+      <c r="N36" s="297">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O36" s="280"/>
+      <c r="O36" s="279"/>
       <c r="P36" s="102"/>
     </row>
     <row r="37" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="70"/>
       <c r="D37" s="72"/>
-      <c r="F37" s="308" t="s">
+      <c r="F37" s="313" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="308"/>
+      <c r="G37" s="313"/>
       <c r="H37" s="73">
         <f>SUM(H5:H30)</f>
         <v>60036.020000000004</v>
@@ -5651,31 +5805,31 @@
     </row>
     <row r="38" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="2:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B39" s="249" t="s">
+      <c r="B39" s="248" t="s">
         <v>100</v>
       </c>
-      <c r="C39" s="250"/>
-      <c r="D39" s="251"/>
-      <c r="E39" s="251"/>
-      <c r="F39" s="252"/>
+      <c r="C39" s="249"/>
+      <c r="D39" s="250"/>
+      <c r="E39" s="250"/>
+      <c r="F39" s="251"/>
     </row>
     <row r="40" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="253" t="s">
+      <c r="B40" s="252" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="254"/>
-      <c r="D40" s="255"/>
-      <c r="E40" s="255"/>
-      <c r="F40" s="256"/>
+      <c r="C40" s="253"/>
+      <c r="D40" s="254"/>
+      <c r="E40" s="254"/>
+      <c r="F40" s="255"/>
     </row>
     <row r="41" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="257" t="s">
+      <c r="B41" s="256" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="258"/>
-      <c r="D41" s="259"/>
-      <c r="E41" s="259"/>
-      <c r="F41" s="260"/>
+      <c r="C41" s="257"/>
+      <c r="D41" s="258"/>
+      <c r="E41" s="258"/>
+      <c r="F41" s="259"/>
     </row>
   </sheetData>
   <sortState ref="B5:L27">
@@ -5715,8 +5869,8 @@
   </sheetPr>
   <dimension ref="B1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5740,10 +5894,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="349" t="s">
+      <c r="B1" s="354" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="349"/>
+      <c r="C1" s="354"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -5755,15 +5909,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="300">
+      <c r="B2" s="305">
         <v>44535</v>
       </c>
-      <c r="C2" s="301"/>
-      <c r="F2" s="327" t="s">
+      <c r="C2" s="306"/>
+      <c r="F2" s="332" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="327"/>
-      <c r="H2" s="327"/>
+      <c r="G2" s="332"/>
+      <c r="H2" s="332"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -5773,32 +5927,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="302" t="s">
+      <c r="C3" s="307" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="303"/>
+      <c r="D3" s="308"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="304" t="s">
+      <c r="F3" s="309" t="s">
         <v>94</v>
       </c>
-      <c r="G3" s="305"/>
+      <c r="G3" s="310"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="306" t="s">
+      <c r="I3" s="311" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="313" t="s">
+      <c r="K3" s="318" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="314"/>
-      <c r="M3" s="309" t="s">
+      <c r="L3" s="319"/>
+      <c r="M3" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="310"/>
-      <c r="O3" s="311" t="s">
+      <c r="N3" s="315"/>
+      <c r="O3" s="316" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="312"/>
+      <c r="P3" s="317"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -5817,10 +5971,10 @@
       <c r="G4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="170" t="s">
+      <c r="H4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="307"/>
+      <c r="I4" s="312"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -5843,65 +5997,81 @@
     </row>
     <row r="5" spans="2:24" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="21" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="C5" s="240"/>
       <c r="D5" s="23"/>
       <c r="E5" s="24"/>
-      <c r="F5" s="240"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="174">
+      <c r="F5" s="240">
+        <v>857.02</v>
+      </c>
+      <c r="G5" s="25">
+        <v>67</v>
+      </c>
+      <c r="H5" s="300">
         <f t="shared" ref="H5:I27" si="0">F5+C5</f>
-        <v>0</v>
+        <v>857.02</v>
       </c>
       <c r="I5" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="J5" s="28"/>
-      <c r="K5" s="207"/>
-      <c r="L5" s="208"/>
-      <c r="M5" s="281">
+      <c r="K5" s="364">
+        <v>857.02</v>
+      </c>
+      <c r="L5" s="365">
+        <v>67</v>
+      </c>
+      <c r="M5" s="280">
         <f>K5-H5</f>
         <v>0</v>
       </c>
-      <c r="N5" s="282">
+      <c r="N5" s="281">
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="350"/>
-      <c r="P5" s="339"/>
+      <c r="O5" s="355"/>
+      <c r="P5" s="344"/>
     </row>
     <row r="6" spans="2:24" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="C6" s="240"/>
       <c r="D6" s="23"/>
       <c r="E6" s="24"/>
-      <c r="F6" s="240"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="174">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F6" s="240">
+        <v>1059</v>
+      </c>
+      <c r="G6" s="25">
+        <v>39</v>
+      </c>
+      <c r="H6" s="301">
+        <f t="shared" si="0"/>
+        <v>1059</v>
       </c>
       <c r="I6" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="J6" s="28"/>
-      <c r="K6" s="207"/>
-      <c r="L6" s="208"/>
-      <c r="M6" s="283">
+      <c r="K6" s="364">
+        <v>1059</v>
+      </c>
+      <c r="L6" s="365">
+        <v>88</v>
+      </c>
+      <c r="M6" s="282">
         <f t="shared" ref="M6:N22" si="1">K6-H6</f>
         <v>0</v>
       </c>
-      <c r="N6" s="284">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="351"/>
-      <c r="P6" s="331"/>
+      <c r="N6" s="283">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="O6" s="356"/>
+      <c r="P6" s="336"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
       <c r="U6" s="226"/>
@@ -5911,45 +6081,57 @@
     </row>
     <row r="7" spans="2:24" ht="27.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B7" s="21" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="C7" s="240"/>
       <c r="D7" s="23"/>
       <c r="E7" s="24"/>
-      <c r="F7" s="240"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="174">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F7" s="240">
+        <v>120</v>
+      </c>
+      <c r="G7" s="25">
+        <v>6</v>
+      </c>
+      <c r="H7" s="301">
+        <f t="shared" si="0"/>
+        <v>120</v>
       </c>
       <c r="I7" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J7" s="28"/>
-      <c r="K7" s="207"/>
-      <c r="L7" s="208"/>
-      <c r="M7" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N7" s="286">
+      <c r="K7" s="364">
+        <v>120</v>
+      </c>
+      <c r="L7" s="365">
+        <v>6</v>
+      </c>
+      <c r="M7" s="284">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="285">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O7" s="190"/>
       <c r="P7" s="161"/>
     </row>
-    <row r="8" spans="2:24" ht="18" hidden="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:24" ht="34.5" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B8" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="240"/>
-      <c r="D8" s="23"/>
+        <v>106</v>
+      </c>
+      <c r="C8" s="242"/>
+      <c r="D8" s="42"/>
       <c r="E8" s="24"/>
-      <c r="F8" s="240"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="174">
+      <c r="F8" s="240">
+        <v>0</v>
+      </c>
+      <c r="G8" s="25">
+        <v>0</v>
+      </c>
+      <c r="H8" s="301">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5960,235 +6142,307 @@
       <c r="J8" s="28"/>
       <c r="K8" s="207"/>
       <c r="L8" s="208"/>
-      <c r="M8" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="286">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="348"/>
-      <c r="P8" s="343"/>
+      <c r="M8" s="284">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="285">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="353"/>
+      <c r="P8" s="348"/>
     </row>
     <row r="9" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="21" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="C9" s="240"/>
       <c r="D9" s="23"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="240"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="174">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F9" s="240">
+        <v>1493.63</v>
+      </c>
+      <c r="G9" s="25">
+        <v>61</v>
+      </c>
+      <c r="H9" s="301">
+        <f t="shared" si="0"/>
+        <v>1493.63</v>
       </c>
       <c r="I9" s="171">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="J9" s="28"/>
-      <c r="K9" s="207"/>
-      <c r="L9" s="208"/>
-      <c r="M9" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N9" s="286">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="261"/>
+      <c r="K9" s="364">
+        <v>1493.63</v>
+      </c>
+      <c r="L9" s="365">
+        <v>61</v>
+      </c>
+      <c r="M9" s="284">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="285">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="260"/>
       <c r="P9" s="132"/>
     </row>
     <row r="10" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" s="240"/>
       <c r="D10" s="23"/>
       <c r="E10" s="24"/>
-      <c r="F10" s="240"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="174">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F10" s="240">
+        <v>80</v>
+      </c>
+      <c r="G10" s="25">
+        <v>8</v>
+      </c>
+      <c r="H10" s="301">
+        <f t="shared" si="0"/>
+        <v>80</v>
       </c>
       <c r="I10" s="171">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J10" s="28"/>
-      <c r="K10" s="207"/>
-      <c r="L10" s="208"/>
-      <c r="M10" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N10" s="286">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="352"/>
-      <c r="P10" s="333"/>
-    </row>
-    <row r="11" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="164" t="s">
-        <v>69</v>
+      <c r="K10" s="366">
+        <v>80</v>
+      </c>
+      <c r="L10" s="367">
+        <v>8</v>
+      </c>
+      <c r="M10" s="284">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="285">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="357"/>
+      <c r="P10" s="338"/>
+    </row>
+    <row r="11" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="21" t="s">
+        <v>92</v>
       </c>
       <c r="C11" s="240"/>
       <c r="D11" s="23"/>
       <c r="E11" s="24"/>
-      <c r="F11" s="240"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="237">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F11" s="240">
+        <v>30</v>
+      </c>
+      <c r="G11" s="25">
+        <v>3</v>
+      </c>
+      <c r="H11" s="301">
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="I11" s="171">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J11" s="28"/>
-      <c r="K11" s="207"/>
-      <c r="L11" s="208"/>
-      <c r="M11" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="286">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="262"/>
-      <c r="P11" s="248"/>
-    </row>
-    <row r="12" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="240"/>
-      <c r="D12" s="23"/>
+      <c r="K11" s="366">
+        <v>30</v>
+      </c>
+      <c r="L11" s="367">
+        <v>3</v>
+      </c>
+      <c r="M11" s="284">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="285">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="261"/>
+      <c r="P11" s="247"/>
+    </row>
+    <row r="12" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="164" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="240">
+        <v>4041.96</v>
+      </c>
+      <c r="D12" s="23">
+        <v>178</v>
+      </c>
       <c r="E12" s="24"/>
-      <c r="F12" s="240"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="176">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F12" s="240">
+        <v>1581.62</v>
+      </c>
+      <c r="G12" s="25">
+        <v>66</v>
+      </c>
+      <c r="H12" s="299">
+        <f t="shared" si="0"/>
+        <v>5623.58</v>
       </c>
       <c r="I12" s="171">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="J12" s="28"/>
-      <c r="K12" s="212"/>
-      <c r="L12" s="213"/>
-      <c r="M12" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="286">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="263"/>
+      <c r="K12" s="366">
+        <v>5623.58</v>
+      </c>
+      <c r="L12" s="367">
+        <v>244</v>
+      </c>
+      <c r="M12" s="284">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="285">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="262"/>
       <c r="P12" s="136"/>
+      <c r="S12" s="377"/>
+      <c r="T12" s="377"/>
     </row>
     <row r="13" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="21" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C13" s="240"/>
       <c r="D13" s="23"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="240"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="176">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F13" s="240">
+        <v>86.61</v>
+      </c>
+      <c r="G13" s="25">
+        <v>3</v>
+      </c>
+      <c r="H13" s="177">
+        <f t="shared" si="0"/>
+        <v>86.61</v>
       </c>
       <c r="I13" s="171">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J13" s="28"/>
-      <c r="K13" s="212"/>
-      <c r="L13" s="213"/>
-      <c r="M13" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="286">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="264"/>
+      <c r="K13" s="366">
+        <v>86.61</v>
+      </c>
+      <c r="L13" s="367">
+        <v>3</v>
+      </c>
+      <c r="M13" s="284">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="285">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="263"/>
       <c r="P13" s="138"/>
+      <c r="S13" s="377"/>
+      <c r="T13" s="377"/>
     </row>
     <row r="14" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="C14" s="240"/>
       <c r="D14" s="23"/>
       <c r="E14" s="24"/>
-      <c r="F14" s="240"/>
-      <c r="G14" s="25"/>
+      <c r="F14" s="240">
+        <v>19087.009999999998</v>
+      </c>
+      <c r="G14" s="25">
+        <v>579</v>
+      </c>
       <c r="H14" s="176">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19087.009999999998</v>
       </c>
       <c r="I14" s="171">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>579</v>
       </c>
       <c r="J14" s="28"/>
-      <c r="K14" s="212"/>
-      <c r="L14" s="213"/>
-      <c r="M14" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="286">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="353"/>
-      <c r="P14" s="322"/>
-    </row>
-    <row r="15" spans="2:24" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K14" s="212">
+        <v>19086.77</v>
+      </c>
+      <c r="L14" s="213">
+        <v>576</v>
+      </c>
+      <c r="M14" s="302">
+        <f t="shared" si="1"/>
+        <v>-0.23999999999796273</v>
+      </c>
+      <c r="N14" s="303">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="O14" s="358"/>
+      <c r="P14" s="327"/>
+      <c r="Q14" s="381" t="s">
+        <v>107</v>
+      </c>
+      <c r="R14" s="373"/>
+      <c r="S14" s="378"/>
+      <c r="T14" s="377"/>
+    </row>
+    <row r="15" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="21" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="C15" s="240"/>
       <c r="D15" s="23"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="240"/>
-      <c r="G15" s="25"/>
+      <c r="F15" s="240">
+        <v>1002.78</v>
+      </c>
+      <c r="G15" s="25">
+        <v>37</v>
+      </c>
       <c r="H15" s="176">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1002.78</v>
       </c>
       <c r="I15" s="171">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="J15" s="28"/>
-      <c r="K15" s="212"/>
-      <c r="L15" s="213"/>
-      <c r="M15" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="286">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="265"/>
+      <c r="K15" s="366">
+        <v>1003.13</v>
+      </c>
+      <c r="L15" s="367">
+        <v>37</v>
+      </c>
+      <c r="M15" s="284">
+        <f t="shared" si="1"/>
+        <v>0.35000000000002274</v>
+      </c>
+      <c r="N15" s="285">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="264"/>
       <c r="P15" s="140"/>
-    </row>
-    <row r="16" spans="2:24" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S15" s="377"/>
+      <c r="T15" s="377"/>
+    </row>
+    <row r="16" spans="2:24" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="21" t="s">
         <v>87</v>
       </c>
@@ -6208,80 +6462,106 @@
       <c r="J16" s="28"/>
       <c r="K16" s="212"/>
       <c r="L16" s="213"/>
-      <c r="M16" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="286">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="266"/>
+      <c r="M16" s="284">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="285">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="265"/>
       <c r="P16" s="142"/>
-    </row>
-    <row r="17" spans="2:16" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S16" s="377"/>
+      <c r="T16" s="377"/>
+    </row>
+    <row r="17" spans="2:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>
       <c r="C17" s="240"/>
       <c r="D17" s="23"/>
       <c r="E17" s="24"/>
-      <c r="F17" s="240"/>
-      <c r="G17" s="25"/>
+      <c r="F17" s="240">
+        <v>863.3</v>
+      </c>
+      <c r="G17" s="25">
+        <v>46</v>
+      </c>
       <c r="H17" s="176">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>863.3</v>
       </c>
       <c r="I17" s="171">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="J17" s="28"/>
-      <c r="K17" s="212"/>
-      <c r="L17" s="213"/>
-      <c r="M17" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="286">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="267"/>
+      <c r="K17" s="366">
+        <v>863.3</v>
+      </c>
+      <c r="L17" s="367">
+        <v>46</v>
+      </c>
+      <c r="M17" s="284">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="285">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="266"/>
       <c r="P17" s="144"/>
-    </row>
-    <row r="18" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S17" s="377"/>
+      <c r="T17" s="377"/>
+    </row>
+    <row r="18" spans="2:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="240"/>
-      <c r="D18" s="23"/>
+      <c r="C18" s="240">
+        <v>172.53</v>
+      </c>
+      <c r="D18" s="23">
+        <v>38</v>
+      </c>
       <c r="E18" s="24"/>
-      <c r="F18" s="240"/>
-      <c r="G18" s="25"/>
+      <c r="F18" s="240">
+        <v>2043</v>
+      </c>
+      <c r="G18" s="25">
+        <v>450</v>
+      </c>
       <c r="H18" s="176">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2215.5300000000002</v>
       </c>
       <c r="I18" s="171">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>488</v>
       </c>
       <c r="J18" s="28"/>
-      <c r="K18" s="212"/>
-      <c r="L18" s="213"/>
-      <c r="M18" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="286">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="268"/>
+      <c r="K18" s="366">
+        <v>2215.52</v>
+      </c>
+      <c r="L18" s="367">
+        <v>488</v>
+      </c>
+      <c r="M18" s="284">
+        <f t="shared" si="1"/>
+        <v>-1.0000000000218279E-2</v>
+      </c>
+      <c r="N18" s="285">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="267"/>
       <c r="P18" s="146"/>
-    </row>
-    <row r="19" spans="2:16" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S18" s="377"/>
+      <c r="T18" s="377"/>
+    </row>
+    <row r="19" spans="2:20" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="163" t="s">
         <v>50</v>
       </c>
@@ -6301,113 +6581,153 @@
       <c r="J19" s="5"/>
       <c r="K19" s="212"/>
       <c r="L19" s="213"/>
-      <c r="M19" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="286">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="354"/>
-      <c r="P19" s="324"/>
-    </row>
-    <row r="20" spans="2:16" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M19" s="284">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="285">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="359"/>
+      <c r="P19" s="329"/>
+      <c r="S19" s="377"/>
+      <c r="T19" s="377"/>
+    </row>
+    <row r="20" spans="2:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="240"/>
-      <c r="D20" s="23"/>
+        <v>23</v>
+      </c>
+      <c r="C20" s="240">
+        <v>4417.28</v>
+      </c>
+      <c r="D20" s="23">
+        <v>152</v>
+      </c>
       <c r="E20" s="24"/>
       <c r="F20" s="240"/>
       <c r="G20" s="25"/>
       <c r="H20" s="176">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4417.28</v>
       </c>
       <c r="I20" s="171">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="J20" s="28"/>
-      <c r="K20" s="212"/>
-      <c r="L20" s="213"/>
-      <c r="M20" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="286">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="269"/>
+      <c r="K20" s="366">
+        <v>4400.83</v>
+      </c>
+      <c r="L20" s="367">
+        <v>151</v>
+      </c>
+      <c r="M20" s="302">
+        <f t="shared" si="1"/>
+        <v>-16.449999999999818</v>
+      </c>
+      <c r="N20" s="303">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="O20" s="268"/>
       <c r="P20" s="148"/>
-    </row>
-    <row r="21" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q20" s="380" t="s">
+        <v>107</v>
+      </c>
+      <c r="R20" s="376"/>
+      <c r="S20" s="379"/>
+      <c r="T20" s="377"/>
+    </row>
+    <row r="21" spans="2:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="21" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="C21" s="240"/>
       <c r="D21" s="23"/>
       <c r="E21" s="24"/>
-      <c r="F21" s="240"/>
-      <c r="G21" s="25"/>
+      <c r="F21" s="240">
+        <v>4550</v>
+      </c>
+      <c r="G21" s="25">
+        <v>350</v>
+      </c>
       <c r="H21" s="176">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4550</v>
       </c>
       <c r="I21" s="171">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="J21" s="28"/>
-      <c r="K21" s="212"/>
-      <c r="L21" s="213"/>
-      <c r="M21" s="285">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="286">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="355"/>
-      <c r="P21" s="329"/>
-    </row>
-    <row r="22" spans="2:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K21" s="212">
+        <v>4771</v>
+      </c>
+      <c r="L21" s="213">
+        <v>367</v>
+      </c>
+      <c r="M21" s="284">
+        <f t="shared" si="1"/>
+        <v>221</v>
+      </c>
+      <c r="N21" s="285">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="O21" s="360"/>
+      <c r="P21" s="334"/>
+      <c r="Q21" s="380" t="s">
+        <v>107</v>
+      </c>
+      <c r="R21" s="372"/>
+      <c r="S21" s="371"/>
+      <c r="T21" s="377"/>
+    </row>
+    <row r="22" spans="2:20" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="240"/>
-      <c r="D22" s="23"/>
+      <c r="C22" s="240">
+        <v>18863.46</v>
+      </c>
+      <c r="D22" s="23">
+        <v>693</v>
+      </c>
       <c r="E22" s="24"/>
       <c r="F22" s="240"/>
       <c r="G22" s="25"/>
       <c r="H22" s="176">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18863.46</v>
       </c>
       <c r="I22" s="171">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>693</v>
       </c>
       <c r="J22" s="28"/>
-      <c r="K22" s="212"/>
-      <c r="L22" s="213"/>
-      <c r="M22" s="287">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="288">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="356"/>
-      <c r="P22" s="357"/>
-    </row>
-    <row r="23" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K22" s="366">
+        <v>18862.419999999998</v>
+      </c>
+      <c r="L22" s="367">
+        <v>693</v>
+      </c>
+      <c r="M22" s="286">
+        <f t="shared" si="1"/>
+        <v>-1.0400000000008731</v>
+      </c>
+      <c r="N22" s="287">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="361"/>
+      <c r="P22" s="362"/>
+      <c r="S22" s="377"/>
+      <c r="T22" s="377"/>
+    </row>
+    <row r="23" spans="2:20" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C23" s="240"/>
       <c r="D23" s="23"/>
@@ -6425,51 +6745,59 @@
       <c r="J23" s="28"/>
       <c r="K23" s="216"/>
       <c r="L23" s="217"/>
-      <c r="M23" s="285">
+      <c r="M23" s="284">
         <f t="shared" ref="M23:N36" si="2">K23-H23</f>
         <v>0</v>
       </c>
-      <c r="N23" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="270"/>
+      <c r="N23" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="269"/>
       <c r="P23" s="192"/>
     </row>
-    <row r="24" spans="2:16" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="240"/>
-      <c r="D24" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="C24" s="240">
+        <v>910.15</v>
+      </c>
+      <c r="D24" s="23">
+        <v>43</v>
+      </c>
       <c r="E24" s="24"/>
       <c r="F24" s="240"/>
       <c r="G24" s="25"/>
       <c r="H24" s="176">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>910.15</v>
       </c>
       <c r="I24" s="171">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="J24" s="28"/>
-      <c r="K24" s="216"/>
-      <c r="L24" s="217"/>
-      <c r="M24" s="285">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N24" s="286">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O24" s="271"/>
+      <c r="K24" s="368">
+        <v>909.4</v>
+      </c>
+      <c r="L24" s="369">
+        <v>43</v>
+      </c>
+      <c r="M24" s="284">
+        <f t="shared" si="2"/>
+        <v>-0.75</v>
+      </c>
+      <c r="N24" s="285">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="270"/>
       <c r="P24" s="194"/>
     </row>
-    <row r="25" spans="2:16" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:20" ht="23.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C25" s="240"/>
       <c r="D25" s="23"/>
@@ -6487,23 +6815,23 @@
       <c r="J25" s="28"/>
       <c r="K25" s="218"/>
       <c r="L25" s="213"/>
-      <c r="M25" s="289">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N25" s="290">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O25" s="358"/>
-      <c r="P25" s="337"/>
-    </row>
-    <row r="26" spans="2:16" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M25" s="288">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="289">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="363"/>
+      <c r="P25" s="342"/>
+    </row>
+    <row r="26" spans="2:20" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="240"/>
-      <c r="D26" s="23"/>
+        <v>29</v>
+      </c>
+      <c r="C26" s="241"/>
+      <c r="D26" s="298"/>
       <c r="E26" s="24"/>
       <c r="F26" s="245"/>
       <c r="G26" s="48"/>
@@ -6518,23 +6846,23 @@
       <c r="J26" s="28"/>
       <c r="K26" s="218"/>
       <c r="L26" s="213"/>
-      <c r="M26" s="291">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N26" s="292">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O26" s="272"/>
+      <c r="M26" s="290">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="291">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="271"/>
       <c r="P26" s="196"/>
     </row>
-    <row r="27" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="241"/>
-      <c r="D27" s="247"/>
+    <row r="27" spans="2:20" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="163" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="240"/>
+      <c r="D27" s="23"/>
       <c r="E27" s="24"/>
       <c r="F27" s="245"/>
       <c r="G27" s="48"/>
@@ -6549,23 +6877,23 @@
       <c r="J27" s="28"/>
       <c r="K27" s="218"/>
       <c r="L27" s="213"/>
-      <c r="M27" s="291">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N27" s="292">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O27" s="273"/>
+      <c r="M27" s="290">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="291">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="272"/>
       <c r="P27" s="96"/>
     </row>
-    <row r="28" spans="2:16" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="163" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="240"/>
-      <c r="D28" s="23"/>
+    <row r="28" spans="2:20" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="242"/>
+      <c r="D28" s="42"/>
       <c r="E28" s="24"/>
       <c r="F28" s="245"/>
       <c r="G28" s="48"/>
@@ -6580,20 +6908,20 @@
       <c r="J28" s="28"/>
       <c r="K28" s="218"/>
       <c r="L28" s="213"/>
-      <c r="M28" s="291">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N28" s="292">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O28" s="273"/>
+      <c r="M28" s="290">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="291">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O28" s="272"/>
       <c r="P28" s="96"/>
     </row>
-    <row r="29" spans="2:16" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:20" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="21" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C29" s="242"/>
       <c r="D29" s="42"/>
@@ -6611,23 +6939,23 @@
       <c r="J29" s="28"/>
       <c r="K29" s="218"/>
       <c r="L29" s="213"/>
-      <c r="M29" s="291">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N29" s="292">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O29" s="274"/>
+      <c r="M29" s="290">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="291">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="273"/>
       <c r="P29" s="98"/>
     </row>
-    <row r="30" spans="2:16" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="243"/>
-      <c r="D30" s="167"/>
+        <v>25</v>
+      </c>
+      <c r="C30" s="246"/>
+      <c r="D30" s="53"/>
       <c r="E30" s="54"/>
       <c r="F30" s="246"/>
       <c r="G30" s="56"/>
@@ -6640,53 +6968,65 @@
         <v>0</v>
       </c>
       <c r="J30" s="28"/>
-      <c r="K30" s="218"/>
-      <c r="L30" s="213"/>
-      <c r="M30" s="291">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N30" s="292">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O30" s="275"/>
+      <c r="K30" s="370">
+        <v>0</v>
+      </c>
+      <c r="L30" s="367">
+        <v>0</v>
+      </c>
+      <c r="M30" s="290">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="291">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="274"/>
       <c r="P30" s="93"/>
     </row>
-    <row r="31" spans="2:16" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="165" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="242"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="115"/>
-      <c r="F31" s="246"/>
-      <c r="G31" s="60"/>
+    <row r="31" spans="2:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="182" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="240"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="246">
+        <v>99.88</v>
+      </c>
+      <c r="G31" s="60">
+        <v>22</v>
+      </c>
       <c r="H31" s="178">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>99.88</v>
       </c>
       <c r="I31" s="173">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J31" s="28"/>
-      <c r="K31" s="218"/>
-      <c r="L31" s="213"/>
-      <c r="M31" s="291">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N31" s="292">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O31" s="276"/>
+      <c r="K31" s="370">
+        <v>99.88</v>
+      </c>
+      <c r="L31" s="367">
+        <v>22</v>
+      </c>
+      <c r="M31" s="290">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="291">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="275"/>
       <c r="P31" s="100"/>
     </row>
-    <row r="32" spans="2:16" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="182" t="s">
-        <v>66</v>
+    <row r="32" spans="2:20" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="162" t="s">
+        <v>52</v>
       </c>
       <c r="C32" s="240"/>
       <c r="D32" s="23"/>
@@ -6704,80 +7044,96 @@
       <c r="J32" s="28"/>
       <c r="K32" s="218"/>
       <c r="L32" s="213"/>
-      <c r="M32" s="293">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N32" s="294">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O32" s="277"/>
+      <c r="M32" s="292">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="293">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O32" s="276"/>
       <c r="P32" s="198"/>
     </row>
-    <row r="33" spans="2:16" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="162" t="s">
-        <v>52</v>
+    <row r="33" spans="2:17" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="165" t="s">
+        <v>101</v>
       </c>
       <c r="C33" s="240"/>
       <c r="D33" s="23"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="246"/>
-      <c r="G33" s="60"/>
+      <c r="E33" s="115"/>
+      <c r="F33" s="246">
+        <v>549.76</v>
+      </c>
+      <c r="G33" s="60">
+        <v>45</v>
+      </c>
       <c r="H33" s="178">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>549.76</v>
       </c>
       <c r="I33" s="173">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J33" s="28"/>
-      <c r="K33" s="218"/>
-      <c r="L33" s="213"/>
-      <c r="M33" s="289">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N33" s="290">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O33" s="278"/>
+      <c r="K33" s="370">
+        <v>549.76</v>
+      </c>
+      <c r="L33" s="367">
+        <v>45</v>
+      </c>
+      <c r="M33" s="288">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N33" s="289">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O33" s="277"/>
       <c r="P33" s="232"/>
     </row>
-    <row r="34" spans="2:16" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B34" s="165" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="240"/>
       <c r="D34" s="23"/>
       <c r="E34" s="115"/>
-      <c r="F34" s="246"/>
-      <c r="G34" s="60"/>
+      <c r="F34" s="246">
+        <v>402.05</v>
+      </c>
+      <c r="G34" s="60">
+        <v>19</v>
+      </c>
       <c r="H34" s="178">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>402.05</v>
       </c>
       <c r="I34" s="173">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J34" s="28"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="121"/>
-      <c r="M34" s="295">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N34" s="296">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O34" s="279"/>
+      <c r="K34" s="370">
+        <v>402.05</v>
+      </c>
+      <c r="L34" s="367">
+        <v>19</v>
+      </c>
+      <c r="M34" s="294">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N34" s="295">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O34" s="278"/>
       <c r="P34" s="200"/>
     </row>
-    <row r="35" spans="2:16" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:17" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="183" t="s">
         <v>32</v>
       </c>
@@ -6797,18 +7153,18 @@
       <c r="J35" s="28"/>
       <c r="K35" s="43"/>
       <c r="L35" s="121"/>
-      <c r="M35" s="295">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N35" s="296">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O35" s="276"/>
+      <c r="M35" s="294">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N35" s="295">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O35" s="275"/>
       <c r="P35" s="100"/>
     </row>
-    <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="68"/>
       <c r="C36" s="22"/>
       <c r="D36" s="23"/>
@@ -6826,72 +7182,83 @@
       <c r="J36" s="28"/>
       <c r="K36" s="69"/>
       <c r="L36" s="179"/>
-      <c r="M36" s="297">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N36" s="298">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O36" s="280"/>
+      <c r="M36" s="296">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N36" s="297">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O36" s="279"/>
       <c r="P36" s="102"/>
     </row>
-    <row r="37" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="70"/>
       <c r="D37" s="72"/>
-      <c r="F37" s="308" t="s">
+      <c r="F37" s="313" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="308"/>
+      <c r="G37" s="313"/>
       <c r="H37" s="73">
         <f>SUM(H5:H30)</f>
-        <v>0</v>
+        <v>61259.35</v>
       </c>
       <c r="I37" s="74">
         <f>SUM(I5:I30)</f>
-        <v>0</v>
+        <v>2819</v>
       </c>
       <c r="J37" s="75"/>
       <c r="K37" s="76">
         <f>SUM(K5:K35)</f>
-        <v>0</v>
+        <v>62513.9</v>
       </c>
       <c r="L37" s="117">
         <f>SUM(L5:L35)</f>
-        <v>0</v>
+        <v>2967</v>
       </c>
       <c r="O37" s="78"/>
     </row>
-    <row r="38" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="2:16" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B39" s="249" t="s">
-        <v>100</v>
-      </c>
-      <c r="C39" s="250"/>
-      <c r="D39" s="251"/>
-      <c r="E39" s="251"/>
-      <c r="F39" s="252"/>
-    </row>
-    <row r="40" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="253" t="s">
-        <v>98</v>
-      </c>
-      <c r="C40" s="254"/>
-      <c r="D40" s="255"/>
-      <c r="E40" s="255"/>
-      <c r="F40" s="256"/>
-    </row>
-    <row r="41" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="257" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" s="258"/>
-      <c r="D41" s="259"/>
-      <c r="E41" s="259"/>
-      <c r="F41" s="260"/>
+    <row r="39" spans="2:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="375"/>
+      <c r="C39" s="374"/>
+      <c r="D39" s="382" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" s="383"/>
+      <c r="F39" s="383"/>
+      <c r="G39" s="384"/>
+      <c r="H39" s="385"/>
+      <c r="I39" s="385"/>
+      <c r="J39" s="385"/>
+      <c r="K39" s="385"/>
+      <c r="L39" s="386"/>
+      <c r="M39" s="387"/>
+      <c r="N39" s="388"/>
+      <c r="O39" s="385"/>
+      <c r="P39" s="389"/>
+      <c r="Q39" s="385"/>
+    </row>
+    <row r="40" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="375"/>
+      <c r="C40" s="374"/>
+      <c r="D40" s="375"/>
+      <c r="E40" s="375"/>
+      <c r="F40" s="375"/>
+      <c r="G40" s="156"/>
+    </row>
+    <row r="41" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="375"/>
+      <c r="C41" s="374"/>
+      <c r="D41" s="375"/>
+      <c r="E41" s="375"/>
+      <c r="F41" s="375"/>
+      <c r="G41" s="156"/>
     </row>
   </sheetData>
+  <sortState ref="B5:G34">
+    <sortCondition ref="B5:B34"/>
+  </sortState>
   <mergeCells count="19">
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="O10:P10"/>
@@ -6900,11 +7267,6 @@
     <mergeCell ref="O21:P21"/>
     <mergeCell ref="O22:P22"/>
     <mergeCell ref="O25:P25"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -6912,9 +7274,14 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I3:I4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.19685039370078741" top="0.39370078740157483" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="90" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -6962,10 +7329,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="299" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="299"/>
+      <c r="A1" s="304" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="304"/>
       <c r="G1" s="156"/>
       <c r="H1" s="157"/>
       <c r="I1" s="157"/>
@@ -6977,10 +7344,10 @@
       <c r="O1" s="161"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="300" t="s">
+      <c r="A2" s="305" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="301"/>
+      <c r="B2" s="306"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -6994,32 +7361,32 @@
     </row>
     <row r="3" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
-      <c r="B3" s="302" t="s">
+      <c r="B3" s="307" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="303"/>
+      <c r="C3" s="308"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="304" t="s">
+      <c r="E3" s="309" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="305"/>
+      <c r="F3" s="310"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="306" t="s">
+      <c r="H3" s="311" t="s">
         <v>2</v>
       </c>
       <c r="I3" s="11"/>
-      <c r="J3" s="313" t="s">
+      <c r="J3" s="318" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="314"/>
-      <c r="L3" s="309" t="s">
+      <c r="K3" s="319"/>
+      <c r="L3" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="310"/>
-      <c r="N3" s="311" t="s">
+      <c r="M3" s="315"/>
+      <c r="N3" s="316" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="312"/>
+      <c r="O3" s="317"/>
     </row>
     <row r="4" spans="1:15" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
@@ -7041,7 +7408,7 @@
       <c r="G4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="307"/>
+      <c r="H4" s="312"/>
       <c r="I4" s="11"/>
       <c r="J4" s="16" t="s">
         <v>10</v>
@@ -7304,8 +7671,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N11" s="321"/>
-      <c r="O11" s="322"/>
+      <c r="N11" s="326"/>
+      <c r="O11" s="327"/>
     </row>
     <row r="12" spans="1:15" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
@@ -7475,8 +7842,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N16" s="323"/>
-      <c r="O16" s="324"/>
+      <c r="N16" s="328"/>
+      <c r="O16" s="329"/>
     </row>
     <row r="17" spans="1:15" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
@@ -7553,8 +7920,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N18" s="325"/>
-      <c r="O18" s="326"/>
+      <c r="N18" s="330"/>
+      <c r="O18" s="331"/>
     </row>
     <row r="19" spans="1:15" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
@@ -8030,10 +8397,10 @@
     <row r="34" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="70"/>
       <c r="C34" s="72"/>
-      <c r="E34" s="308" t="s">
+      <c r="E34" s="313" t="s">
         <v>34</v>
       </c>
-      <c r="F34" s="308"/>
+      <c r="F34" s="313"/>
       <c r="G34" s="73">
         <f>SUM(G5:G27)</f>
         <v>37848.980000000003</v>
@@ -8109,10 +8476,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="299" t="s">
+      <c r="B1" s="304" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="299"/>
+      <c r="C1" s="304"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -8124,15 +8491,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="300" t="s">
+      <c r="B2" s="305" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="301"/>
-      <c r="F2" s="327" t="s">
+      <c r="C2" s="306"/>
+      <c r="F2" s="332" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="327"/>
-      <c r="H2" s="327"/>
+      <c r="G2" s="332"/>
+      <c r="H2" s="332"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -8142,32 +8509,32 @@
     </row>
     <row r="3" spans="2:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="302" t="s">
+      <c r="C3" s="307" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="303"/>
+      <c r="D3" s="308"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="304" t="s">
+      <c r="F3" s="309" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="305"/>
+      <c r="G3" s="310"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="306" t="s">
+      <c r="I3" s="311" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="313" t="s">
+      <c r="K3" s="318" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="314"/>
-      <c r="M3" s="309" t="s">
+      <c r="L3" s="319"/>
+      <c r="M3" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="310"/>
-      <c r="O3" s="311" t="s">
+      <c r="N3" s="315"/>
+      <c r="O3" s="316" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="312"/>
+      <c r="P3" s="317"/>
     </row>
     <row r="4" spans="2:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -8189,7 +8556,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="307"/>
+      <c r="I4" s="312"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -8440,8 +8807,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O11" s="321"/>
-      <c r="P11" s="322"/>
+      <c r="O11" s="326"/>
+      <c r="P11" s="327"/>
     </row>
     <row r="12" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="21" t="s">
@@ -8611,8 +8978,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O16" s="323"/>
-      <c r="P16" s="324"/>
+      <c r="O16" s="328"/>
+      <c r="P16" s="329"/>
     </row>
     <row r="17" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
@@ -8681,8 +9048,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="325"/>
-      <c r="P18" s="326"/>
+      <c r="O18" s="330"/>
+      <c r="P18" s="331"/>
     </row>
     <row r="19" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
@@ -9157,10 +9524,10 @@
     <row r="33" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="70"/>
       <c r="D33" s="72"/>
-      <c r="F33" s="308" t="s">
+      <c r="F33" s="313" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="308"/>
+      <c r="G33" s="313"/>
       <c r="H33" s="73">
         <f>SUM(H5:H26)</f>
         <v>36939.64</v>
@@ -9237,10 +9604,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="299" t="s">
+      <c r="B1" s="304" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="299"/>
+      <c r="C1" s="304"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -9252,15 +9619,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="300" t="s">
+      <c r="B2" s="305" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="301"/>
-      <c r="F2" s="327" t="s">
+      <c r="C2" s="306"/>
+      <c r="F2" s="332" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="327"/>
-      <c r="H2" s="327"/>
+      <c r="G2" s="332"/>
+      <c r="H2" s="332"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -9270,32 +9637,32 @@
     </row>
     <row r="3" spans="2:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="302" t="s">
+      <c r="C3" s="307" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="303"/>
+      <c r="D3" s="308"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="304" t="s">
+      <c r="F3" s="309" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="305"/>
+      <c r="G3" s="310"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="306" t="s">
+      <c r="I3" s="311" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="313" t="s">
+      <c r="K3" s="318" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="314"/>
-      <c r="M3" s="309" t="s">
+      <c r="L3" s="319"/>
+      <c r="M3" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="310"/>
-      <c r="O3" s="311" t="s">
+      <c r="N3" s="315"/>
+      <c r="O3" s="316" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="312"/>
+      <c r="P3" s="317"/>
     </row>
     <row r="4" spans="2:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -9317,7 +9684,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="307"/>
+      <c r="I4" s="312"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -9576,8 +9943,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O11" s="321"/>
-      <c r="P11" s="322"/>
+      <c r="O11" s="326"/>
+      <c r="P11" s="327"/>
     </row>
     <row r="12" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="21" t="s">
@@ -9747,8 +10114,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O16" s="323"/>
-      <c r="P16" s="324"/>
+      <c r="O16" s="328"/>
+      <c r="P16" s="329"/>
     </row>
     <row r="17" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
@@ -9809,8 +10176,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="325"/>
-      <c r="P18" s="326"/>
+      <c r="O18" s="330"/>
+      <c r="P18" s="331"/>
     </row>
     <row r="19" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
@@ -10320,10 +10687,10 @@
     <row r="34" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="70"/>
       <c r="D34" s="72"/>
-      <c r="F34" s="308" t="s">
+      <c r="F34" s="313" t="s">
         <v>34</v>
       </c>
-      <c r="G34" s="308"/>
+      <c r="G34" s="313"/>
       <c r="H34" s="73">
         <f>SUM(H5:H27)</f>
         <v>42297.960000000006</v>
@@ -10400,10 +10767,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="299" t="s">
+      <c r="B1" s="304" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="299"/>
+      <c r="C1" s="304"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -10415,15 +10782,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="300" t="s">
+      <c r="B2" s="305" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="301"/>
-      <c r="F2" s="327" t="s">
+      <c r="C2" s="306"/>
+      <c r="F2" s="332" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="327"/>
-      <c r="H2" s="327"/>
+      <c r="G2" s="332"/>
+      <c r="H2" s="332"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -10433,32 +10800,32 @@
     </row>
     <row r="3" spans="2:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="302" t="s">
+      <c r="C3" s="307" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="303"/>
+      <c r="D3" s="308"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="304" t="s">
+      <c r="F3" s="309" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="305"/>
+      <c r="G3" s="310"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="306" t="s">
+      <c r="I3" s="311" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="313" t="s">
+      <c r="K3" s="318" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="314"/>
-      <c r="M3" s="309" t="s">
+      <c r="L3" s="319"/>
+      <c r="M3" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="310"/>
-      <c r="O3" s="311" t="s">
+      <c r="N3" s="315"/>
+      <c r="O3" s="316" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="312"/>
+      <c r="P3" s="317"/>
     </row>
     <row r="4" spans="2:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -10480,7 +10847,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="307"/>
+      <c r="I4" s="312"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -10533,10 +10900,10 @@
         <f>L5-I5</f>
         <v>-1</v>
       </c>
-      <c r="O5" s="338" t="s">
+      <c r="O5" s="343" t="s">
         <v>71</v>
       </c>
-      <c r="P5" s="339"/>
+      <c r="P5" s="344"/>
     </row>
     <row r="6" spans="2:16" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -10574,10 +10941,10 @@
         <f t="shared" ref="N6:N9" si="2">L6-I6</f>
         <v>-20</v>
       </c>
-      <c r="O6" s="330" t="s">
+      <c r="O6" s="335" t="s">
         <v>70</v>
       </c>
-      <c r="P6" s="331"/>
+      <c r="P6" s="336"/>
     </row>
     <row r="7" spans="2:16" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="21" t="s">
@@ -10654,10 +11021,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O8" s="340" t="s">
+      <c r="O8" s="345" t="s">
         <v>80</v>
       </c>
-      <c r="P8" s="341"/>
+      <c r="P8" s="346"/>
     </row>
     <row r="9" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="164" t="s">
@@ -10730,10 +11097,10 @@
         <f t="shared" ref="N10" si="4">L10-I10</f>
         <v>-1</v>
       </c>
-      <c r="O10" s="332" t="s">
+      <c r="O10" s="337" t="s">
         <v>71</v>
       </c>
-      <c r="P10" s="333"/>
+      <c r="P10" s="338"/>
     </row>
     <row r="11" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="21" t="s">
@@ -10849,8 +11216,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O13" s="321"/>
-      <c r="P13" s="322"/>
+      <c r="O13" s="326"/>
+      <c r="P13" s="327"/>
     </row>
     <row r="14" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
@@ -11020,8 +11387,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O18" s="323"/>
-      <c r="P18" s="324"/>
+      <c r="O18" s="328"/>
+      <c r="P18" s="329"/>
     </row>
     <row r="19" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
@@ -11090,8 +11457,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O20" s="328"/>
-      <c r="P20" s="329"/>
+      <c r="O20" s="333"/>
+      <c r="P20" s="334"/>
     </row>
     <row r="21" spans="2:16" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="21" t="s">
@@ -11133,10 +11500,10 @@
         <f t="shared" si="5"/>
         <v>-4</v>
       </c>
-      <c r="O21" s="334" t="s">
+      <c r="O21" s="339" t="s">
         <v>73</v>
       </c>
-      <c r="P21" s="335"/>
+      <c r="P21" s="340"/>
     </row>
     <row r="22" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
@@ -11240,10 +11607,10 @@
         <f t="shared" si="5"/>
         <v>-21</v>
       </c>
-      <c r="O24" s="336" t="s">
+      <c r="O24" s="341" t="s">
         <v>72</v>
       </c>
-      <c r="P24" s="337"/>
+      <c r="P24" s="342"/>
     </row>
     <row r="25" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="21" t="s">
@@ -11526,10 +11893,10 @@
         <f t="shared" si="6"/>
         <v>-1</v>
       </c>
-      <c r="O32" s="334" t="s">
+      <c r="O32" s="339" t="s">
         <v>74</v>
       </c>
-      <c r="P32" s="335"/>
+      <c r="P32" s="340"/>
     </row>
     <row r="33" spans="2:16" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="B33" s="165" t="s">
@@ -11625,10 +11992,10 @@
     <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="70"/>
       <c r="D36" s="72"/>
-      <c r="F36" s="308" t="s">
+      <c r="F36" s="313" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="308"/>
+      <c r="G36" s="313"/>
       <c r="H36" s="73">
         <f>SUM(H5:H29)</f>
         <v>55685.099999999991</v>
@@ -11712,10 +12079,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="299" t="s">
+      <c r="B1" s="304" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="299"/>
+      <c r="C1" s="304"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -11727,15 +12094,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="300" t="s">
+      <c r="B2" s="305" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="301"/>
-      <c r="F2" s="327" t="s">
+      <c r="C2" s="306"/>
+      <c r="F2" s="332" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="327"/>
-      <c r="H2" s="327"/>
+      <c r="G2" s="332"/>
+      <c r="H2" s="332"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -11745,32 +12112,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="302" t="s">
+      <c r="C3" s="307" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="303"/>
+      <c r="D3" s="308"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="304" t="s">
+      <c r="F3" s="309" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="305"/>
+      <c r="G3" s="310"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="306" t="s">
+      <c r="I3" s="311" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="313" t="s">
+      <c r="K3" s="318" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="314"/>
-      <c r="M3" s="309" t="s">
+      <c r="L3" s="319"/>
+      <c r="M3" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="310"/>
-      <c r="O3" s="311" t="s">
+      <c r="N3" s="315"/>
+      <c r="O3" s="316" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="312"/>
+      <c r="P3" s="317"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -11792,7 +12159,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="307"/>
+      <c r="I4" s="312"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -11841,8 +12208,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="338"/>
-      <c r="P5" s="339"/>
+      <c r="O5" s="343"/>
+      <c r="P5" s="344"/>
     </row>
     <row r="6" spans="2:24" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -11880,8 +12247,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="330"/>
-      <c r="P6" s="331"/>
+      <c r="O6" s="335"/>
+      <c r="P6" s="336"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
       <c r="U6" s="226"/>
@@ -11968,8 +12335,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="342"/>
-      <c r="P8" s="343"/>
+      <c r="O8" s="347"/>
+      <c r="P8" s="348"/>
     </row>
     <row r="9" spans="2:24" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="164" t="s">
@@ -12030,10 +12397,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="332" t="s">
+      <c r="O10" s="337" t="s">
         <v>71</v>
       </c>
-      <c r="P10" s="333"/>
+      <c r="P10" s="338"/>
     </row>
     <row r="11" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="21" t="s">
@@ -12153,8 +12520,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="321"/>
-      <c r="P13" s="322"/>
+      <c r="O13" s="326"/>
+      <c r="P13" s="327"/>
     </row>
     <row r="14" spans="2:24" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="21" t="s">
@@ -12324,8 +12691,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="323"/>
-      <c r="P18" s="324"/>
+      <c r="O18" s="328"/>
+      <c r="P18" s="329"/>
     </row>
     <row r="19" spans="2:16" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="21" t="s">
@@ -12394,8 +12761,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="328"/>
-      <c r="P20" s="329"/>
+      <c r="O20" s="333"/>
+      <c r="P20" s="334"/>
     </row>
     <row r="21" spans="2:16" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="21" t="s">
@@ -12437,10 +12804,10 @@
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
-      <c r="O21" s="334" t="s">
+      <c r="O21" s="339" t="s">
         <v>79</v>
       </c>
-      <c r="P21" s="335"/>
+      <c r="P21" s="340"/>
     </row>
     <row r="22" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
@@ -12548,8 +12915,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="336"/>
-      <c r="P24" s="337"/>
+      <c r="O24" s="341"/>
+      <c r="P24" s="342"/>
     </row>
     <row r="25" spans="2:16" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="21" t="s">
@@ -12820,10 +13187,10 @@
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="O32" s="334" t="s">
+      <c r="O32" s="339" t="s">
         <v>78</v>
       </c>
-      <c r="P32" s="335"/>
+      <c r="P32" s="340"/>
     </row>
     <row r="33" spans="2:16" ht="17.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="B33" s="165" t="s">
@@ -12919,10 +13286,10 @@
     <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="70"/>
       <c r="D36" s="72"/>
-      <c r="F36" s="308" t="s">
+      <c r="F36" s="313" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="308"/>
+      <c r="G36" s="313"/>
       <c r="H36" s="73">
         <f>SUM(H5:H29)</f>
         <v>56083.79800000001</v>
@@ -13003,10 +13370,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="299" t="s">
+      <c r="B1" s="304" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="299"/>
+      <c r="C1" s="304"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -13018,15 +13385,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="300" t="s">
+      <c r="B2" s="305" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="301"/>
-      <c r="F2" s="327" t="s">
+      <c r="C2" s="306"/>
+      <c r="F2" s="332" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="327"/>
-      <c r="H2" s="327"/>
+      <c r="G2" s="332"/>
+      <c r="H2" s="332"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -13036,32 +13403,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="302" t="s">
+      <c r="C3" s="307" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="303"/>
+      <c r="D3" s="308"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="304" t="s">
+      <c r="F3" s="309" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="305"/>
+      <c r="G3" s="310"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="306" t="s">
+      <c r="I3" s="311" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="313" t="s">
+      <c r="K3" s="318" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="314"/>
-      <c r="M3" s="309" t="s">
+      <c r="L3" s="319"/>
+      <c r="M3" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="310"/>
-      <c r="O3" s="311" t="s">
+      <c r="N3" s="315"/>
+      <c r="O3" s="316" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="312"/>
+      <c r="P3" s="317"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -13083,7 +13450,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="307"/>
+      <c r="I4" s="312"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -13132,8 +13499,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="338"/>
-      <c r="P5" s="339"/>
+      <c r="O5" s="343"/>
+      <c r="P5" s="344"/>
     </row>
     <row r="6" spans="2:24" ht="39" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -13163,8 +13530,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="330"/>
-      <c r="P6" s="331"/>
+      <c r="O6" s="335"/>
+      <c r="P6" s="336"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
       <c r="U6" s="226"/>
@@ -13239,8 +13606,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="342"/>
-      <c r="P8" s="343"/>
+      <c r="O8" s="347"/>
+      <c r="P8" s="348"/>
     </row>
     <row r="9" spans="2:24" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="164" t="s">
@@ -13305,10 +13672,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="332" t="s">
+      <c r="O10" s="337" t="s">
         <v>71</v>
       </c>
-      <c r="P10" s="333"/>
+      <c r="P10" s="338"/>
     </row>
     <row r="11" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="21" t="s">
@@ -13424,8 +13791,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="321"/>
-      <c r="P13" s="322"/>
+      <c r="O13" s="326"/>
+      <c r="P13" s="327"/>
     </row>
     <row r="14" spans="2:24" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
@@ -13595,8 +13962,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="323"/>
-      <c r="P18" s="324"/>
+      <c r="O18" s="328"/>
+      <c r="P18" s="329"/>
     </row>
     <row r="19" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
@@ -13665,8 +14032,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="328"/>
-      <c r="P20" s="329"/>
+      <c r="O20" s="333"/>
+      <c r="P20" s="334"/>
     </row>
     <row r="21" spans="2:16" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="21" t="s">
@@ -13704,10 +14071,10 @@
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
-      <c r="O21" s="334" t="s">
+      <c r="O21" s="339" t="s">
         <v>79</v>
       </c>
-      <c r="P21" s="335"/>
+      <c r="P21" s="340"/>
     </row>
     <row r="22" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
@@ -13811,8 +14178,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="336"/>
-      <c r="P24" s="337"/>
+      <c r="O24" s="341"/>
+      <c r="P24" s="342"/>
     </row>
     <row r="25" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="21" t="s">
@@ -14075,10 +14442,10 @@
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="O32" s="334" t="s">
+      <c r="O32" s="339" t="s">
         <v>78</v>
       </c>
-      <c r="P32" s="335"/>
+      <c r="P32" s="340"/>
     </row>
     <row r="33" spans="2:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B33" s="165" t="s">
@@ -14174,10 +14541,10 @@
     <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="70"/>
       <c r="D36" s="72"/>
-      <c r="F36" s="308" t="s">
+      <c r="F36" s="313" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="308"/>
+      <c r="G36" s="313"/>
       <c r="H36" s="73">
         <f>SUM(H5:H29)</f>
         <v>23272.91</v>
@@ -14258,10 +14625,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="299" t="s">
+      <c r="B1" s="304" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="299"/>
+      <c r="C1" s="304"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -14273,15 +14640,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="300">
+      <c r="B2" s="305">
         <v>44444</v>
       </c>
-      <c r="C2" s="301"/>
-      <c r="F2" s="327" t="s">
+      <c r="C2" s="306"/>
+      <c r="F2" s="332" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="327"/>
-      <c r="H2" s="327"/>
+      <c r="G2" s="332"/>
+      <c r="H2" s="332"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -14291,32 +14658,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="302" t="s">
+      <c r="C3" s="307" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="303"/>
+      <c r="D3" s="308"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="304" t="s">
+      <c r="F3" s="309" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="305"/>
+      <c r="G3" s="310"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="306" t="s">
+      <c r="I3" s="311" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="313" t="s">
+      <c r="K3" s="318" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="314"/>
-      <c r="M3" s="309" t="s">
+      <c r="L3" s="319"/>
+      <c r="M3" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="310"/>
-      <c r="O3" s="311" t="s">
+      <c r="N3" s="315"/>
+      <c r="O3" s="316" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="312"/>
+      <c r="P3" s="317"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -14338,7 +14705,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="307"/>
+      <c r="I4" s="312"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -14387,8 +14754,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="338"/>
-      <c r="P5" s="339"/>
+      <c r="O5" s="343"/>
+      <c r="P5" s="344"/>
     </row>
     <row r="6" spans="2:24" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -14426,8 +14793,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="330"/>
-      <c r="P6" s="331"/>
+      <c r="O6" s="335"/>
+      <c r="P6" s="336"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
       <c r="U6" s="226"/>
@@ -14502,8 +14869,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="342"/>
-      <c r="P8" s="343"/>
+      <c r="O8" s="347"/>
+      <c r="P8" s="348"/>
     </row>
     <row r="9" spans="2:24" ht="24" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="164" t="s">
@@ -14564,10 +14931,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="332" t="s">
+      <c r="O10" s="337" t="s">
         <v>71</v>
       </c>
-      <c r="P10" s="333"/>
+      <c r="P10" s="338"/>
     </row>
     <row r="11" spans="2:24" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="21" t="s">
@@ -14683,8 +15050,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O13" s="321"/>
-      <c r="P13" s="322"/>
+      <c r="O13" s="326"/>
+      <c r="P13" s="327"/>
     </row>
     <row r="14" spans="2:24" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
@@ -14862,8 +15229,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O18" s="323"/>
-      <c r="P18" s="324"/>
+      <c r="O18" s="328"/>
+      <c r="P18" s="329"/>
     </row>
     <row r="19" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
@@ -14932,8 +15299,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O20" s="328"/>
-      <c r="P20" s="329"/>
+      <c r="O20" s="333"/>
+      <c r="P20" s="334"/>
     </row>
     <row r="21" spans="2:16" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="21" t="s">
@@ -14971,10 +15338,10 @@
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
-      <c r="O21" s="344" t="s">
+      <c r="O21" s="349" t="s">
         <v>88</v>
       </c>
-      <c r="P21" s="345"/>
+      <c r="P21" s="350"/>
     </row>
     <row r="22" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
@@ -15078,8 +15445,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O24" s="336"/>
-      <c r="P24" s="337"/>
+      <c r="O24" s="341"/>
+      <c r="P24" s="342"/>
     </row>
     <row r="25" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="21" t="s">
@@ -15439,10 +15806,10 @@
     <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="70"/>
       <c r="D36" s="72"/>
-      <c r="F36" s="308" t="s">
+      <c r="F36" s="313" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="308"/>
+      <c r="G36" s="313"/>
       <c r="H36" s="73">
         <f>SUM(H5:H29)</f>
         <v>32951.5</v>
@@ -15525,10 +15892,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="299" t="s">
+      <c r="B1" s="304" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="299"/>
+      <c r="C1" s="304"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -15540,15 +15907,15 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="300">
+      <c r="B2" s="305">
         <v>44472</v>
       </c>
-      <c r="C2" s="301"/>
-      <c r="F2" s="327" t="s">
+      <c r="C2" s="306"/>
+      <c r="F2" s="332" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="327"/>
-      <c r="H2" s="327"/>
+      <c r="G2" s="332"/>
+      <c r="H2" s="332"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="2"/>
@@ -15558,32 +15925,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="302" t="s">
+      <c r="C3" s="307" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="303"/>
+      <c r="D3" s="308"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="304" t="s">
+      <c r="F3" s="309" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="305"/>
+      <c r="G3" s="310"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="306" t="s">
+      <c r="I3" s="311" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="313" t="s">
+      <c r="K3" s="318" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="314"/>
-      <c r="M3" s="309" t="s">
+      <c r="L3" s="319"/>
+      <c r="M3" s="314" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="310"/>
-      <c r="O3" s="311" t="s">
+      <c r="N3" s="315"/>
+      <c r="O3" s="316" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="312"/>
+      <c r="P3" s="317"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -15605,7 +15972,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="307"/>
+      <c r="I4" s="312"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -15654,8 +16021,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="338"/>
-      <c r="P5" s="339"/>
+      <c r="O5" s="343"/>
+      <c r="P5" s="344"/>
     </row>
     <row r="6" spans="2:24" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
@@ -15693,8 +16060,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O6" s="330"/>
-      <c r="P6" s="331"/>
+      <c r="O6" s="335"/>
+      <c r="P6" s="336"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
       <c r="U6" s="226"/>
@@ -15769,8 +16136,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="342"/>
-      <c r="P8" s="343"/>
+      <c r="O8" s="347"/>
+      <c r="P8" s="348"/>
     </row>
     <row r="9" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="21" t="s">
@@ -15847,8 +16214,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="332"/>
-      <c r="P10" s="333"/>
+      <c r="O10" s="337"/>
+      <c r="P10" s="338"/>
     </row>
     <row r="11" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="164" t="s">
@@ -15999,8 +16366,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O14" s="321"/>
-      <c r="P14" s="322"/>
+      <c r="O14" s="326"/>
+      <c r="P14" s="327"/>
     </row>
     <row r="15" spans="2:24" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="21" t="s">
@@ -16170,8 +16537,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O19" s="323"/>
-      <c r="P19" s="324"/>
+      <c r="O19" s="328"/>
+      <c r="P19" s="329"/>
     </row>
     <row r="20" spans="2:18" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="21" t="s">
@@ -16232,8 +16599,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="328"/>
-      <c r="P21" s="329"/>
+      <c r="O21" s="333"/>
+      <c r="P21" s="334"/>
     </row>
     <row r="22" spans="2:18" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
@@ -16275,14 +16642,14 @@
         <f t="shared" si="1"/>
         <v>-4</v>
       </c>
-      <c r="O22" s="334" t="s">
+      <c r="O22" s="339" t="s">
         <v>88</v>
       </c>
-      <c r="P22" s="335"/>
-      <c r="Q22" s="346" t="s">
+      <c r="P22" s="340"/>
+      <c r="Q22" s="351" t="s">
         <v>95</v>
       </c>
-      <c r="R22" s="347"/>
+      <c r="R22" s="352"/>
     </row>
     <row r="23" spans="2:18" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="21" t="s">
@@ -16322,8 +16689,8 @@
       </c>
       <c r="O23" s="191"/>
       <c r="P23" s="192"/>
-      <c r="Q23" s="346"/>
-      <c r="R23" s="347"/>
+      <c r="Q23" s="351"/>
+      <c r="R23" s="352"/>
     </row>
     <row r="24" spans="2:18" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="21" t="s">
@@ -16384,8 +16751,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O25" s="336"/>
-      <c r="P25" s="337"/>
+      <c r="O25" s="341"/>
+      <c r="P25" s="342"/>
     </row>
     <row r="26" spans="2:18" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="21" t="s">
@@ -16753,10 +17120,10 @@
     <row r="37" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="70"/>
       <c r="D37" s="72"/>
-      <c r="F37" s="308" t="s">
+      <c r="F37" s="313" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="308"/>
+      <c r="G37" s="313"/>
       <c r="H37" s="73">
         <f>SUM(H5:H30)</f>
         <v>61770.95</v>

</xml_diff>

<commit_message>
CIERRE DEL 11 DE NOV 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/INVENTARIO ALMACEN  NOVIEMBRE        2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/INVENTARIO ALMACEN  NOVIEMBRE        2021.xlsx
@@ -2865,6 +2865,33 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2904,33 +2931,6 @@
     <xf numFmtId="0" fontId="14" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3012,6 +3012,18 @@
     <xf numFmtId="0" fontId="31" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3031,18 +3043,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3408,10 +3408,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="343" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="343"/>
+      <c r="A1" s="330" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="330"/>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -3421,10 +3421,10 @@
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="344" t="s">
+      <c r="A2" s="331" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="345"/>
+      <c r="B2" s="332"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -3438,32 +3438,32 @@
     </row>
     <row r="3" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
-      <c r="B3" s="346" t="s">
+      <c r="B3" s="333" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="347"/>
+      <c r="C3" s="334"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="348" t="s">
+      <c r="E3" s="335" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="349"/>
+      <c r="F3" s="336"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="337" t="s">
         <v>2</v>
       </c>
       <c r="I3" s="11"/>
-      <c r="J3" s="335" t="s">
+      <c r="J3" s="344" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="336"/>
-      <c r="L3" s="331" t="s">
+      <c r="K3" s="345"/>
+      <c r="L3" s="340" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="332"/>
-      <c r="N3" s="333" t="s">
+      <c r="M3" s="341"/>
+      <c r="N3" s="342" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="334"/>
+      <c r="O3" s="343"/>
     </row>
     <row r="4" spans="1:15" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
@@ -3485,7 +3485,7 @@
       <c r="G4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="351"/>
+      <c r="H4" s="338"/>
       <c r="I4" s="11"/>
       <c r="J4" s="16" t="s">
         <v>10</v>
@@ -3758,10 +3758,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N11" s="337" t="s">
+      <c r="N11" s="346" t="s">
         <v>40</v>
       </c>
-      <c r="O11" s="338"/>
+      <c r="O11" s="347"/>
     </row>
     <row r="12" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
@@ -3931,10 +3931,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N16" s="339" t="s">
+      <c r="N16" s="348" t="s">
         <v>41</v>
       </c>
-      <c r="O16" s="340"/>
+      <c r="O16" s="349"/>
     </row>
     <row r="17" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
@@ -4011,10 +4011,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N18" s="341" t="s">
+      <c r="N18" s="350" t="s">
         <v>42</v>
       </c>
-      <c r="O18" s="342"/>
+      <c r="O18" s="351"/>
     </row>
     <row r="19" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
@@ -4510,10 +4510,10 @@
     <row r="34" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="70"/>
       <c r="C34" s="72"/>
-      <c r="E34" s="330" t="s">
+      <c r="E34" s="339" t="s">
         <v>34</v>
       </c>
-      <c r="F34" s="330"/>
+      <c r="F34" s="339"/>
       <c r="G34" s="73">
         <f>SUM(G5:G27)</f>
         <v>68686.460000000006</v>
@@ -4538,11 +4538,6 @@
     <sortCondition ref="A10:A28"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="H3:H4"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
@@ -4550,6 +4545,11 @@
     <mergeCell ref="N11:O11"/>
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="N18:O18"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="H3:H4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.15748031496062992" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4589,10 +4589,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="387" t="s">
+      <c r="B1" s="380" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="387"/>
+      <c r="C1" s="380"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -4604,10 +4604,10 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="344">
+      <c r="B2" s="331">
         <v>44507</v>
       </c>
-      <c r="C2" s="345"/>
+      <c r="C2" s="332"/>
       <c r="F2" s="358" t="s">
         <v>1</v>
       </c>
@@ -4622,32 +4622,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="346" t="s">
+      <c r="C3" s="333" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="347"/>
+      <c r="D3" s="334"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="348" t="s">
+      <c r="F3" s="335" t="s">
         <v>94</v>
       </c>
-      <c r="G3" s="349"/>
+      <c r="G3" s="336"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="350" t="s">
+      <c r="I3" s="337" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="335" t="s">
+      <c r="K3" s="344" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="336"/>
-      <c r="M3" s="331" t="s">
+      <c r="L3" s="345"/>
+      <c r="M3" s="340" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="332"/>
-      <c r="O3" s="333" t="s">
+      <c r="N3" s="341"/>
+      <c r="O3" s="342" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="334"/>
+      <c r="P3" s="343"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -4669,7 +4669,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="351"/>
+      <c r="I4" s="338"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -4726,7 +4726,7 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="388"/>
+      <c r="O5" s="381"/>
       <c r="P5" s="370"/>
     </row>
     <row r="6" spans="2:24" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4765,7 +4765,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O6" s="389"/>
+      <c r="O6" s="382"/>
       <c r="P6" s="362"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
@@ -4841,7 +4841,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O8" s="386"/>
+      <c r="O8" s="379"/>
       <c r="P8" s="374"/>
     </row>
     <row r="9" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -4919,7 +4919,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O10" s="379"/>
+      <c r="O10" s="383"/>
       <c r="P10" s="364"/>
     </row>
     <row r="11" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5075,7 +5075,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O14" s="380"/>
+      <c r="O14" s="384"/>
       <c r="P14" s="353"/>
     </row>
     <row r="15" spans="2:24" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5238,7 +5238,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O19" s="381"/>
+      <c r="O19" s="385"/>
       <c r="P19" s="355"/>
     </row>
     <row r="20" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5308,7 +5308,7 @@
         <f t="shared" si="2"/>
         <v>162</v>
       </c>
-      <c r="O21" s="382"/>
+      <c r="O21" s="386"/>
       <c r="P21" s="360"/>
     </row>
     <row r="22" spans="2:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5347,8 +5347,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O22" s="383"/>
-      <c r="P22" s="384"/>
+      <c r="O22" s="387"/>
+      <c r="P22" s="388"/>
     </row>
     <row r="23" spans="2:16" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="21" t="s">
@@ -5448,7 +5448,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O25" s="385"/>
+      <c r="O25" s="389"/>
       <c r="P25" s="368"/>
     </row>
     <row r="26" spans="2:16" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5801,10 +5801,10 @@
     <row r="37" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="70"/>
       <c r="D37" s="72"/>
-      <c r="F37" s="330" t="s">
+      <c r="F37" s="339" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="330"/>
+      <c r="G37" s="339"/>
       <c r="H37" s="73">
         <f>SUM(H5:H30)</f>
         <v>60036.020000000004</v>
@@ -5857,6 +5857,13 @@
     <sortCondition ref="B5:B27"/>
   </sortState>
   <mergeCells count="19">
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O25:P25"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -5869,13 +5876,6 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O25:P25"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.47244094488188981" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5890,8 +5890,8 @@
   </sheetPr>
   <dimension ref="B1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5915,10 +5915,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="387" t="s">
+      <c r="B1" s="380" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="387"/>
+      <c r="C1" s="380"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -5948,32 +5948,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="346" t="s">
+      <c r="C3" s="333" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="347"/>
+      <c r="D3" s="334"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="348" t="s">
+      <c r="F3" s="335" t="s">
         <v>110</v>
       </c>
-      <c r="G3" s="349"/>
+      <c r="G3" s="336"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="350" t="s">
+      <c r="I3" s="337" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="335" t="s">
+      <c r="K3" s="344" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="336"/>
-      <c r="M3" s="331" t="s">
+      <c r="L3" s="345"/>
+      <c r="M3" s="340" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="332"/>
-      <c r="O3" s="333" t="s">
+      <c r="N3" s="341"/>
+      <c r="O3" s="342" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="334"/>
+      <c r="P3" s="343"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -5995,7 +5995,7 @@
       <c r="H4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="351"/>
+      <c r="I4" s="338"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -6052,7 +6052,7 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="388"/>
+      <c r="O5" s="381"/>
       <c r="P5" s="370"/>
     </row>
     <row r="6" spans="2:24" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6066,7 +6066,7 @@
         <v>1059</v>
       </c>
       <c r="G6" s="25">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="H6" s="301">
         <f t="shared" si="0"/>
@@ -6074,7 +6074,7 @@
       </c>
       <c r="I6" s="27">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="J6" s="28"/>
       <c r="K6" s="304">
@@ -6089,9 +6089,9 @@
       </c>
       <c r="N6" s="283">
         <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
-      <c r="O6" s="389"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="382"/>
       <c r="P6" s="362"/>
       <c r="S6" s="224"/>
       <c r="T6" s="225"/>
@@ -6171,7 +6171,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="386"/>
+      <c r="O8" s="379"/>
       <c r="P8" s="374"/>
     </row>
     <row r="9" spans="2:24" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -6249,7 +6249,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="379"/>
+      <c r="O10" s="383"/>
       <c r="P10" s="364"/>
     </row>
     <row r="11" spans="2:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -6413,7 +6413,7 @@
         <f t="shared" si="1"/>
         <v>-3</v>
       </c>
-      <c r="O14" s="380"/>
+      <c r="O14" s="384"/>
       <c r="P14" s="353"/>
       <c r="Q14" s="321" t="s">
         <v>107</v>
@@ -6610,7 +6610,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O19" s="381"/>
+      <c r="O19" s="385"/>
       <c r="P19" s="355"/>
       <c r="S19" s="317"/>
       <c r="T19" s="317"/>
@@ -6696,7 +6696,7 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="O21" s="382"/>
+      <c r="O21" s="386"/>
       <c r="P21" s="360"/>
       <c r="Q21" s="320" t="s">
         <v>107</v>
@@ -6741,8 +6741,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O22" s="383"/>
-      <c r="P22" s="384"/>
+      <c r="O22" s="387"/>
+      <c r="P22" s="388"/>
       <c r="S22" s="317"/>
       <c r="T22" s="317"/>
     </row>
@@ -6844,7 +6844,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O25" s="385"/>
+      <c r="O25" s="389"/>
       <c r="P25" s="368"/>
     </row>
     <row r="26" spans="2:20" ht="24" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7217,17 +7217,17 @@
     <row r="37" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="70"/>
       <c r="D37" s="72"/>
-      <c r="F37" s="330" t="s">
+      <c r="F37" s="339" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="330"/>
+      <c r="G37" s="339"/>
       <c r="H37" s="73">
         <f>SUM(H5:H30)</f>
         <v>61259.35</v>
       </c>
       <c r="I37" s="74">
         <f>SUM(I5:I30)</f>
-        <v>2819</v>
+        <v>2868</v>
       </c>
       <c r="J37" s="75"/>
       <c r="K37" s="76">
@@ -7281,6 +7281,13 @@
     <sortCondition ref="B5:B34"/>
   </sortState>
   <mergeCells count="19">
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O25:P25"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -7293,13 +7300,6 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O25:P25"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.19685039370078741" top="0.39370078740157483" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7350,10 +7350,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="343" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="343"/>
+      <c r="A1" s="330" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="330"/>
       <c r="G1" s="156"/>
       <c r="H1" s="157"/>
       <c r="I1" s="157"/>
@@ -7365,10 +7365,10 @@
       <c r="O1" s="161"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="344" t="s">
+      <c r="A2" s="331" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="345"/>
+      <c r="B2" s="332"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -7382,32 +7382,32 @@
     </row>
     <row r="3" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
-      <c r="B3" s="346" t="s">
+      <c r="B3" s="333" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="347"/>
+      <c r="C3" s="334"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="348" t="s">
+      <c r="E3" s="335" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="349"/>
+      <c r="F3" s="336"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="337" t="s">
         <v>2</v>
       </c>
       <c r="I3" s="11"/>
-      <c r="J3" s="335" t="s">
+      <c r="J3" s="344" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="336"/>
-      <c r="L3" s="331" t="s">
+      <c r="K3" s="345"/>
+      <c r="L3" s="340" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="332"/>
-      <c r="N3" s="333" t="s">
+      <c r="M3" s="341"/>
+      <c r="N3" s="342" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="334"/>
+      <c r="O3" s="343"/>
     </row>
     <row r="4" spans="1:15" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
@@ -7429,7 +7429,7 @@
       <c r="G4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="351"/>
+      <c r="H4" s="338"/>
       <c r="I4" s="11"/>
       <c r="J4" s="16" t="s">
         <v>10</v>
@@ -8418,10 +8418,10 @@
     <row r="34" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="70"/>
       <c r="C34" s="72"/>
-      <c r="E34" s="330" t="s">
+      <c r="E34" s="339" t="s">
         <v>34</v>
       </c>
-      <c r="F34" s="330"/>
+      <c r="F34" s="339"/>
       <c r="G34" s="73">
         <f>SUM(G5:G27)</f>
         <v>37848.980000000003</v>
@@ -8446,11 +8446,6 @@
     <sortCondition ref="A6:A28"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N18:O18"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="E34:F34"/>
@@ -8458,6 +8453,11 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N18:O18"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.15748031496062992" top="0.39370078740157483" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -8497,10 +8497,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="343" t="s">
+      <c r="B1" s="330" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="343"/>
+      <c r="C1" s="330"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -8512,10 +8512,10 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="344" t="s">
+      <c r="B2" s="331" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="345"/>
+      <c r="C2" s="332"/>
       <c r="F2" s="358" t="s">
         <v>1</v>
       </c>
@@ -8530,32 +8530,32 @@
     </row>
     <row r="3" spans="2:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="346" t="s">
+      <c r="C3" s="333" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="347"/>
+      <c r="D3" s="334"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="348" t="s">
+      <c r="F3" s="335" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="349"/>
+      <c r="G3" s="336"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="350" t="s">
+      <c r="I3" s="337" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="335" t="s">
+      <c r="K3" s="344" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="336"/>
-      <c r="M3" s="331" t="s">
+      <c r="L3" s="345"/>
+      <c r="M3" s="340" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="332"/>
-      <c r="O3" s="333" t="s">
+      <c r="N3" s="341"/>
+      <c r="O3" s="342" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="334"/>
+      <c r="P3" s="343"/>
     </row>
     <row r="4" spans="2:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -8577,7 +8577,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="351"/>
+      <c r="I4" s="338"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -9545,10 +9545,10 @@
     <row r="33" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="70"/>
       <c r="D33" s="72"/>
-      <c r="F33" s="330" t="s">
+      <c r="F33" s="339" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="330"/>
+      <c r="G33" s="339"/>
       <c r="H33" s="73">
         <f>SUM(H5:H26)</f>
         <v>36939.64</v>
@@ -9573,6 +9573,11 @@
     <sortCondition ref="B27:B30"/>
   </sortState>
   <mergeCells count="13">
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O18:P18"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="F2:H2"/>
@@ -9581,11 +9586,6 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O18:P18"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.15748031496062992" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -9625,10 +9625,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="343" t="s">
+      <c r="B1" s="330" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="343"/>
+      <c r="C1" s="330"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -9640,10 +9640,10 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="344" t="s">
+      <c r="B2" s="331" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="345"/>
+      <c r="C2" s="332"/>
       <c r="F2" s="358" t="s">
         <v>1</v>
       </c>
@@ -9658,32 +9658,32 @@
     </row>
     <row r="3" spans="2:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="346" t="s">
+      <c r="C3" s="333" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="347"/>
+      <c r="D3" s="334"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="348" t="s">
+      <c r="F3" s="335" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="349"/>
+      <c r="G3" s="336"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="350" t="s">
+      <c r="I3" s="337" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="335" t="s">
+      <c r="K3" s="344" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="336"/>
-      <c r="M3" s="331" t="s">
+      <c r="L3" s="345"/>
+      <c r="M3" s="340" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="332"/>
-      <c r="O3" s="333" t="s">
+      <c r="N3" s="341"/>
+      <c r="O3" s="342" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="334"/>
+      <c r="P3" s="343"/>
     </row>
     <row r="4" spans="2:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -9705,7 +9705,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="351"/>
+      <c r="I4" s="338"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -10708,10 +10708,10 @@
     <row r="34" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="70"/>
       <c r="D34" s="72"/>
-      <c r="F34" s="330" t="s">
+      <c r="F34" s="339" t="s">
         <v>34</v>
       </c>
-      <c r="G34" s="330"/>
+      <c r="G34" s="339"/>
       <c r="H34" s="73">
         <f>SUM(H5:H27)</f>
         <v>42297.960000000006</v>
@@ -10736,11 +10736,6 @@
     <sortCondition ref="B6:B31"/>
   </sortState>
   <mergeCells count="13">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
@@ -10749,6 +10744,11 @@
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="O18:P18"/>
     <mergeCell ref="I3:I4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.16" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -10788,10 +10788,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="343" t="s">
+      <c r="B1" s="330" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="343"/>
+      <c r="C1" s="330"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -10803,10 +10803,10 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="344" t="s">
+      <c r="B2" s="331" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="345"/>
+      <c r="C2" s="332"/>
       <c r="F2" s="358" t="s">
         <v>1</v>
       </c>
@@ -10821,32 +10821,32 @@
     </row>
     <row r="3" spans="2:16" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="346" t="s">
+      <c r="C3" s="333" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="347"/>
+      <c r="D3" s="334"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="348" t="s">
+      <c r="F3" s="335" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="349"/>
+      <c r="G3" s="336"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="350" t="s">
+      <c r="I3" s="337" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="335" t="s">
+      <c r="K3" s="344" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="336"/>
-      <c r="M3" s="331" t="s">
+      <c r="L3" s="345"/>
+      <c r="M3" s="340" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="332"/>
-      <c r="O3" s="333" t="s">
+      <c r="N3" s="341"/>
+      <c r="O3" s="342" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="334"/>
+      <c r="P3" s="343"/>
     </row>
     <row r="4" spans="2:16" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -10868,7 +10868,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="351"/>
+      <c r="I4" s="338"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -12013,10 +12013,10 @@
     <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="70"/>
       <c r="D36" s="72"/>
-      <c r="F36" s="330" t="s">
+      <c r="F36" s="339" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="330"/>
+      <c r="G36" s="339"/>
       <c r="H36" s="73">
         <f>SUM(H5:H29)</f>
         <v>55685.099999999991</v>
@@ -12041,6 +12041,11 @@
     <sortCondition ref="B5:B34"/>
   </sortState>
   <mergeCells count="20">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
@@ -12056,11 +12061,6 @@
     <mergeCell ref="O32:P32"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O8:P8"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -12100,10 +12100,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="343" t="s">
+      <c r="B1" s="330" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="343"/>
+      <c r="C1" s="330"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -12115,10 +12115,10 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="344" t="s">
+      <c r="B2" s="331" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="345"/>
+      <c r="C2" s="332"/>
       <c r="F2" s="358" t="s">
         <v>1</v>
       </c>
@@ -12133,32 +12133,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="346" t="s">
+      <c r="C3" s="333" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="347"/>
+      <c r="D3" s="334"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="348" t="s">
+      <c r="F3" s="335" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="349"/>
+      <c r="G3" s="336"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="350" t="s">
+      <c r="I3" s="337" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="335" t="s">
+      <c r="K3" s="344" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="336"/>
-      <c r="M3" s="331" t="s">
+      <c r="L3" s="345"/>
+      <c r="M3" s="340" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="332"/>
-      <c r="O3" s="333" t="s">
+      <c r="N3" s="341"/>
+      <c r="O3" s="342" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="334"/>
+      <c r="P3" s="343"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -12180,7 +12180,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="351"/>
+      <c r="I4" s="338"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -13307,10 +13307,10 @@
     <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="70"/>
       <c r="D36" s="72"/>
-      <c r="F36" s="330" t="s">
+      <c r="F36" s="339" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="330"/>
+      <c r="G36" s="339"/>
       <c r="H36" s="73">
         <f>SUM(H5:H29)</f>
         <v>56083.79800000001</v>
@@ -13332,14 +13332,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O24:P24"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -13352,6 +13344,14 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O24:P24"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.15748031496062992" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -13391,10 +13391,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="343" t="s">
+      <c r="B1" s="330" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="343"/>
+      <c r="C1" s="330"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -13406,10 +13406,10 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="344" t="s">
+      <c r="B2" s="331" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="345"/>
+      <c r="C2" s="332"/>
       <c r="F2" s="358" t="s">
         <v>1</v>
       </c>
@@ -13424,32 +13424,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="346" t="s">
+      <c r="C3" s="333" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="347"/>
+      <c r="D3" s="334"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="348" t="s">
+      <c r="F3" s="335" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="349"/>
+      <c r="G3" s="336"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="350" t="s">
+      <c r="I3" s="337" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="335" t="s">
+      <c r="K3" s="344" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="336"/>
-      <c r="M3" s="331" t="s">
+      <c r="L3" s="345"/>
+      <c r="M3" s="340" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="332"/>
-      <c r="O3" s="333" t="s">
+      <c r="N3" s="341"/>
+      <c r="O3" s="342" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="334"/>
+      <c r="P3" s="343"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -13471,7 +13471,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="351"/>
+      <c r="I4" s="338"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -14562,10 +14562,10 @@
     <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="70"/>
       <c r="D36" s="72"/>
-      <c r="F36" s="330" t="s">
+      <c r="F36" s="339" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="330"/>
+      <c r="G36" s="339"/>
       <c r="H36" s="73">
         <f>SUM(H5:H29)</f>
         <v>23272.91</v>
@@ -14587,14 +14587,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O24:P24"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -14607,6 +14599,14 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O24:P24"/>
   </mergeCells>
   <pageMargins left="0.27559055118110237" right="0.15748031496062992" top="0.43307086614173229" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14646,10 +14646,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="343" t="s">
+      <c r="B1" s="330" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="343"/>
+      <c r="C1" s="330"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -14661,10 +14661,10 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="344">
+      <c r="B2" s="331">
         <v>44444</v>
       </c>
-      <c r="C2" s="345"/>
+      <c r="C2" s="332"/>
       <c r="F2" s="358" t="s">
         <v>1</v>
       </c>
@@ -14679,32 +14679,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="346" t="s">
+      <c r="C3" s="333" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="347"/>
+      <c r="D3" s="334"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="348" t="s">
+      <c r="F3" s="335" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="349"/>
+      <c r="G3" s="336"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="350" t="s">
+      <c r="I3" s="337" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="335" t="s">
+      <c r="K3" s="344" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="336"/>
-      <c r="M3" s="331" t="s">
+      <c r="L3" s="345"/>
+      <c r="M3" s="340" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="332"/>
-      <c r="O3" s="333" t="s">
+      <c r="N3" s="341"/>
+      <c r="O3" s="342" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="334"/>
+      <c r="P3" s="343"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -14726,7 +14726,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="351"/>
+      <c r="I4" s="338"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -15827,10 +15827,10 @@
     <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="70"/>
       <c r="D36" s="72"/>
-      <c r="F36" s="330" t="s">
+      <c r="F36" s="339" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="330"/>
+      <c r="G36" s="339"/>
       <c r="H36" s="73">
         <f>SUM(H5:H29)</f>
         <v>32951.5</v>
@@ -15855,6 +15855,13 @@
     <sortCondition ref="B15:B18"/>
   </sortState>
   <mergeCells count="19">
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O24:P24"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -15867,13 +15874,6 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O24:P24"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.15748031496062992" top="0.43307086614173229" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -15913,10 +15913,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="343" t="s">
+      <c r="B1" s="330" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="343"/>
+      <c r="C1" s="330"/>
       <c r="H1" s="156"/>
       <c r="I1" s="157"/>
       <c r="J1" s="157"/>
@@ -15928,10 +15928,10 @@
       <c r="P1" s="161"/>
     </row>
     <row r="2" spans="2:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="344">
+      <c r="B2" s="331">
         <v>44472</v>
       </c>
-      <c r="C2" s="345"/>
+      <c r="C2" s="332"/>
       <c r="F2" s="358" t="s">
         <v>1</v>
       </c>
@@ -15946,32 +15946,32 @@
     </row>
     <row r="3" spans="2:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9"/>
-      <c r="C3" s="346" t="s">
+      <c r="C3" s="333" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="347"/>
+      <c r="D3" s="334"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="348" t="s">
+      <c r="F3" s="335" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="349"/>
+      <c r="G3" s="336"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="350" t="s">
+      <c r="I3" s="337" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="335" t="s">
+      <c r="K3" s="344" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="336"/>
-      <c r="M3" s="331" t="s">
+      <c r="L3" s="345"/>
+      <c r="M3" s="340" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="332"/>
-      <c r="O3" s="333" t="s">
+      <c r="N3" s="341"/>
+      <c r="O3" s="342" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="334"/>
+      <c r="P3" s="343"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -15993,7 +15993,7 @@
       <c r="H4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="351"/>
+      <c r="I4" s="338"/>
       <c r="J4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -17141,10 +17141,10 @@
     <row r="37" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="70"/>
       <c r="D37" s="72"/>
-      <c r="F37" s="330" t="s">
+      <c r="F37" s="339" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="330"/>
+      <c r="G37" s="339"/>
       <c r="H37" s="73">
         <f>SUM(H5:H30)</f>
         <v>61770.95</v>
@@ -17169,13 +17169,6 @@
     <sortCondition ref="B9:B11"/>
   </sortState>
   <mergeCells count="20">
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O25:P25"/>
     <mergeCell ref="Q22:R23"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="B1:C1"/>
@@ -17189,6 +17182,13 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="O6:P6"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O25:P25"/>
   </mergeCells>
   <pageMargins left="0.47244094488188981" right="0.15748031496062992" top="0.35433070866141736" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>